<commit_message>
add DMI output to ADX #1262
</commit_message>
<xml_diff>
--- a/tests/indicators/a-d/Adx/Adx.Calc.xlsx
+++ b/tests/indicators/a-d/Adx/Adx.Calc.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1D8B8F-9F53-4B0A-A856-4006463BEA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3415FB2C-712A-4184-A87B-956C4B37A34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36480" yWindow="0" windowWidth="28800" windowHeight="21690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ADX" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -607,7 +598,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1549,22 +1540,22 @@
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="12" max="16" width="9.140625" style="7"/>
-    <col min="17" max="17" width="3.7109375" customWidth="1"/>
-    <col min="18" max="18" width="8.140625" style="5" customWidth="1"/>
-    <col min="19" max="21" width="9.140625" style="7"/>
-    <col min="23" max="23" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="9.140625" style="7"/>
+    <col min="9" max="9" width="9.1796875" customWidth="1"/>
+    <col min="12" max="16" width="9.1796875" style="7"/>
+    <col min="17" max="17" width="3.7265625" customWidth="1"/>
+    <col min="18" max="18" width="8.1796875" style="5" customWidth="1"/>
+    <col min="19" max="21" width="9.1796875" style="7"/>
+    <col min="23" max="23" width="8.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="9.1796875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -1635,7 +1626,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -1674,7 +1665,7 @@
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1722,7 +1713,7 @@
       <c r="X3" s="6"/>
       <c r="Y3" s="6"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -1770,7 +1761,7 @@
       <c r="X4" s="6"/>
       <c r="Y4" s="6"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1818,7 +1809,7 @@
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1866,7 +1857,7 @@
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1914,7 +1905,7 @@
       <c r="X7" s="6"/>
       <c r="Y7" s="6"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1962,7 +1953,7 @@
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -2010,7 +2001,7 @@
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -2058,7 +2049,7 @@
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -2106,7 +2097,7 @@
       <c r="X11" s="6"/>
       <c r="Y11" s="6"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -2154,7 +2145,7 @@
       <c r="X12" s="6"/>
       <c r="Y12" s="6"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -2202,7 +2193,7 @@
       <c r="X13" s="6"/>
       <c r="Y13" s="6"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -2250,7 +2241,7 @@
       <c r="X14" s="6"/>
       <c r="Y14" s="6"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -2298,7 +2289,7 @@
       <c r="X15" s="6"/>
       <c r="Y15" s="6"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -2368,7 +2359,7 @@
       <c r="X16" s="6"/>
       <c r="Y16" s="6"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -2438,7 +2429,7 @@
       <c r="X17" s="6"/>
       <c r="Y17" s="6"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -2508,7 +2499,7 @@
       <c r="X18" s="6"/>
       <c r="Y18" s="6"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -2578,7 +2569,7 @@
       <c r="X19" s="6"/>
       <c r="Y19" s="6"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -2648,7 +2639,7 @@
       <c r="X20" s="6"/>
       <c r="Y20" s="6"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -2696,7 +2687,7 @@
         <f>100*testdata[[#This Row],[-DM14]]/testdata[[#This Row],[TR14]]</f>
         <v>25.012425579421205</v>
       </c>
-      <c r="N21" s="6">
+      <c r="N21" s="11">
         <f>100*ABS(testdata[[#This Row],[+DI14]]-testdata[[#This Row],[-DI14]])/(testdata[[#This Row],[+DI14]]+testdata[[#This Row],[-DI14]])</f>
         <v>8.6351139279442961</v>
       </c>
@@ -2718,7 +2709,7 @@
       <c r="X21" s="11"/>
       <c r="Y21" s="11"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -2788,7 +2779,7 @@
       <c r="X22" s="6"/>
       <c r="Y22" s="6"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -2858,7 +2849,7 @@
       <c r="X23" s="6"/>
       <c r="Y23" s="6"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -2928,7 +2919,7 @@
       <c r="X24" s="6"/>
       <c r="Y24" s="6"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -2998,7 +2989,7 @@
       <c r="X25" s="6"/>
       <c r="Y25" s="6"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -3068,7 +3059,7 @@
       <c r="X26" s="6"/>
       <c r="Y26" s="6"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -3138,7 +3129,7 @@
       <c r="X27" s="6"/>
       <c r="Y27" s="6"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -3208,7 +3199,7 @@
       <c r="X28" s="6"/>
       <c r="Y28" s="6"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -3285,7 +3276,7 @@
       </c>
       <c r="Y29" s="13"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -3362,7 +3353,7 @@
       </c>
       <c r="Y30" s="6"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -3410,7 +3401,7 @@
         <f>100*testdata[[#This Row],[-DM14]]/testdata[[#This Row],[TR14]]</f>
         <v>14.165829841353299</v>
       </c>
-      <c r="N31" s="6">
+      <c r="N31" s="11">
         <f>100*ABS(testdata[[#This Row],[+DI14]]-testdata[[#This Row],[-DI14]])/(testdata[[#This Row],[+DI14]]+testdata[[#This Row],[-DI14]])</f>
         <v>45.659962116806589</v>
       </c>
@@ -3439,7 +3430,7 @@
       </c>
       <c r="Y31" s="11"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -3516,7 +3507,7 @@
       </c>
       <c r="Y32" s="6"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -3593,7 +3584,7 @@
       </c>
       <c r="Y33" s="6"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -3670,7 +3661,7 @@
       </c>
       <c r="Y34" s="6"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>33</v>
       </c>
@@ -3747,7 +3738,7 @@
       </c>
       <c r="Y35" s="6"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -3824,7 +3815,7 @@
       </c>
       <c r="Y36" s="6"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -3901,7 +3892,7 @@
       </c>
       <c r="Y37" s="6"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -3978,7 +3969,7 @@
       </c>
       <c r="Y38" s="6"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -4055,7 +4046,7 @@
       </c>
       <c r="Y39" s="6"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -4132,7 +4123,7 @@
       </c>
       <c r="Y40" s="6"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -4209,7 +4200,7 @@
       </c>
       <c r="Y41" s="6"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -4291,7 +4282,7 @@
         <v>29.1061924422517</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -4373,7 +4364,7 @@
         <v>30.612091066317898</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -4455,7 +4446,7 @@
         <v>31.742940902605799</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -4537,7 +4528,7 @@
         <v>32.910704164193803</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -4619,7 +4610,7 @@
         <v>33.800668233057998</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -4701,7 +4692,7 @@
         <v>34.282530871755498</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -4783,7 +4774,7 @@
         <v>35.203773847973203</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -4865,7 +4856,7 @@
         <v>36.059213754461098</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -4947,7 +4938,7 @@
         <v>36.365003212984099</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -5029,7 +5020,7 @@
         <v>37.142611710382397</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -5111,7 +5102,7 @@
         <v>37.952532158976197</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -5193,7 +5184,7 @@
         <v>38.4561721826583</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -5275,7 +5266,7 @@
         <v>39.044472480502797</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -5357,7 +5348,7 @@
         <v>38.805876785297102</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -5439,7 +5430,7 @@
         <v>38.471016752236899</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A57" s="4">
         <v>55</v>
       </c>
@@ -5521,7 +5512,7 @@
         <v>37.4997691385419</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A58" s="4">
         <v>56</v>
       </c>
@@ -5603,7 +5594,7 @@
         <v>36.665467018523003</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A59" s="4">
         <v>57</v>
       </c>
@@ -5685,7 +5676,7 @@
         <v>36.079144579880399</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A60" s="4">
         <v>58</v>
       </c>
@@ -5767,7 +5758,7 @@
         <v>34.551715527415404</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A61" s="4">
         <v>59</v>
       </c>
@@ -5849,7 +5840,7 @@
         <v>33.344820747917403</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A62" s="4">
         <v>60</v>
       </c>
@@ -5931,7 +5922,7 @@
         <v>32.366541473105897</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A63" s="4">
         <v>61</v>
       </c>
@@ -6013,7 +6004,7 @@
         <v>30.914364787662802</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A64" s="4">
         <v>62</v>
       </c>
@@ -6095,7 +6086,7 @@
         <v>30.357705712508601</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A65" s="4">
         <v>63</v>
       </c>
@@ -6177,7 +6168,7 @@
         <v>29.840807999865401</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A66" s="4">
         <v>64</v>
       </c>
@@ -6259,7 +6250,7 @@
         <v>29.172918215714301</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A67" s="4">
         <v>65</v>
       </c>
@@ -6341,7 +6332,7 @@
         <v>28.1491072195229</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A68" s="4">
         <v>66</v>
       </c>
@@ -6423,7 +6414,7 @@
         <v>26.504759350980599</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A69" s="4">
         <v>67</v>
       </c>
@@ -6505,7 +6496,7 @@
         <v>25.231445672096498</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A70" s="4">
         <v>68</v>
       </c>
@@ -6587,7 +6578,7 @@
         <v>23.7548435583547</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A71" s="4">
         <v>69</v>
       </c>
@@ -6669,7 +6660,7 @@
         <v>22.5885590108646</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A72" s="4">
         <v>70</v>
       </c>
@@ -6751,7 +6742,7 @@
         <v>22.295802015566402</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A73" s="4">
         <v>71</v>
       </c>
@@ -6833,7 +6824,7 @@
         <v>21.349036701747899</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A74" s="4">
         <v>72</v>
       </c>
@@ -6915,7 +6906,7 @@
         <v>20.4698974817737</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A75" s="4">
         <v>73</v>
       </c>
@@ -6997,7 +6988,7 @@
         <v>19.577440110008901</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A76" s="4">
         <v>74</v>
       </c>
@@ -7079,7 +7070,7 @@
         <v>18.364523548171501</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A77" s="4">
         <v>75</v>
       </c>
@@ -7161,7 +7152,7 @@
         <v>17.4385494803442</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A78" s="4">
         <v>76</v>
       </c>
@@ -7243,7 +7234,7 @@
         <v>17.329884510539799</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A79" s="4">
         <v>77</v>
       </c>
@@ -7325,7 +7316,7 @@
         <v>17.4648063151473</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A80" s="4">
         <v>78</v>
       </c>
@@ -7407,7 +7398,7 @@
         <v>17.682948149028899</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A81" s="4">
         <v>79</v>
       </c>
@@ -7489,7 +7480,7 @@
         <v>17.7100214417076</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A82" s="4">
         <v>80</v>
       </c>
@@ -7571,7 +7562,7 @@
         <v>17.799489278081499</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A83" s="4">
         <v>81</v>
       </c>
@@ -7653,7 +7644,7 @@
         <v>17.915875466956699</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A84" s="4">
         <v>82</v>
       </c>
@@ -7735,7 +7726,7 @@
         <v>18.023948356626502</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A85" s="4">
         <v>83</v>
       </c>
@@ -7817,7 +7808,7 @@
         <v>18.1939708200286</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A86" s="4">
         <v>84</v>
       </c>
@@ -7899,7 +7890,7 @@
         <v>18.333775819821199</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A87" s="4">
         <v>85</v>
       </c>
@@ -7981,7 +7972,7 @@
         <v>18.729992570185601</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A88" s="4">
         <v>86</v>
       </c>
@@ -8063,7 +8054,7 @@
         <v>18.943293212509801</v>
       </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A89" s="4">
         <v>87</v>
       </c>
@@ -8145,7 +8136,7 @@
         <v>18.845526482244999</v>
       </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A90" s="4">
         <v>88</v>
       </c>
@@ -8227,7 +8218,7 @@
         <v>18.754743089856301</v>
       </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A91" s="4">
         <v>89</v>
       </c>
@@ -8309,7 +8300,7 @@
         <v>18.760152884100101</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A92" s="4">
         <v>90</v>
       </c>
@@ -8391,7 +8382,7 @@
         <v>19.1669628391214</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A93" s="4">
         <v>91</v>
       </c>
@@ -8473,7 +8464,7 @@
         <v>20.081985790329501</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A94" s="4">
         <v>92</v>
       </c>
@@ -8555,7 +8546,7 @@
         <v>20.836070292675601</v>
       </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A95" s="4">
         <v>93</v>
       </c>
@@ -8637,7 +8628,7 @@
         <v>21.073811681227099</v>
       </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A96" s="4">
         <v>94</v>
       </c>
@@ -8719,7 +8710,7 @@
         <v>21.455839944231698</v>
       </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A97" s="4">
         <v>95</v>
       </c>
@@ -8801,7 +8792,7 @@
         <v>21.2716280780853</v>
       </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A98" s="4">
         <v>96</v>
       </c>
@@ -8883,7 +8874,7 @@
         <v>20.5940638953319</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A99" s="4">
         <v>97</v>
       </c>
@@ -8965,7 +8956,7 @@
         <v>20.167656670205499</v>
       </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A100" s="4">
         <v>98</v>
       </c>
@@ -9047,7 +9038,7 @@
         <v>20.199714171617</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A101" s="4">
         <v>99</v>
       </c>
@@ -9129,7 +9120,7 @@
         <v>20.696337137899501</v>
       </c>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A102" s="4">
         <v>100</v>
       </c>
@@ -9211,7 +9202,7 @@
         <v>21.245861567937698</v>
       </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A103" s="4">
         <v>101</v>
       </c>
@@ -9293,7 +9284,7 @@
         <v>21.6262416569778</v>
       </c>
     </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A104" s="4">
         <v>102</v>
       </c>
@@ -9375,7 +9366,7 @@
         <v>21.085307012226501</v>
       </c>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A105" s="4">
         <v>103</v>
       </c>
@@ -9457,7 +9448,7 @@
         <v>21.049995180387899</v>
       </c>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A106" s="4">
         <v>104</v>
       </c>
@@ -9539,7 +9530,7 @@
         <v>21.672467470452801</v>
       </c>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A107" s="4">
         <v>105</v>
       </c>
@@ -9621,7 +9612,7 @@
         <v>22.330384769091701</v>
       </c>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A108" s="4">
         <v>106</v>
       </c>
@@ -9703,7 +9694,7 @@
         <v>22.191305661936902</v>
       </c>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A109" s="4">
         <v>107</v>
       </c>
@@ -9785,7 +9776,7 @@
         <v>22.017220872573901</v>
       </c>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A110" s="4">
         <v>108</v>
       </c>
@@ -9867,7 +9858,7 @@
         <v>21.448871413869199</v>
       </c>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A111" s="4">
         <v>109</v>
       </c>
@@ -9949,7 +9940,7 @@
         <v>20.1916776939816</v>
       </c>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A112" s="4">
         <v>110</v>
       </c>
@@ -10031,7 +10022,7 @@
         <v>19.208650730890302</v>
       </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A113" s="4">
         <v>111</v>
       </c>
@@ -10113,7 +10104,7 @@
         <v>18.876123557151701</v>
       </c>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A114" s="4">
         <v>112</v>
       </c>
@@ -10195,7 +10186,7 @@
         <v>18.8323775209107</v>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A115" s="4">
         <v>113</v>
       </c>
@@ -10277,7 +10268,7 @@
         <v>18.384938741852299</v>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A116" s="4">
         <v>114</v>
       </c>
@@ -10359,7 +10350,7 @@
         <v>17.880924714904499</v>
       </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A117" s="4">
         <v>115</v>
       </c>
@@ -10441,7 +10432,7 @@
         <v>17.8257912322909</v>
       </c>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A118" s="4">
         <v>116</v>
       </c>
@@ -10523,7 +10514,7 @@
         <v>18.021104841539</v>
       </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A119" s="4">
         <v>117</v>
       </c>
@@ -10605,7 +10596,7 @@
         <v>18.204445089235399</v>
       </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A120" s="4">
         <v>118</v>
       </c>
@@ -10687,7 +10678,7 @@
         <v>18.374689604953399</v>
       </c>
     </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A121" s="4">
         <v>119</v>
       </c>
@@ -10769,7 +10760,7 @@
         <v>18.1374786511679</v>
       </c>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A122" s="4">
         <v>120</v>
       </c>
@@ -10851,7 +10842,7 @@
         <v>18.105568195448399</v>
       </c>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A123" s="4">
         <v>121</v>
       </c>
@@ -10933,7 +10924,7 @@
         <v>17.760763803450999</v>
       </c>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A124" s="4">
         <v>122</v>
       </c>
@@ -11015,7 +11006,7 @@
         <v>16.7507030014878</v>
       </c>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A125" s="4">
         <v>123</v>
       </c>
@@ -11097,7 +11088,7 @@
         <v>16.542459502739199</v>
       </c>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A126" s="4">
         <v>124</v>
       </c>
@@ -11179,7 +11170,7 @@
         <v>16.767764871704099</v>
       </c>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A127" s="4">
         <v>125</v>
       </c>
@@ -11261,7 +11252,7 @@
         <v>16.556801427059099</v>
       </c>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A128" s="4">
         <v>126</v>
       </c>
@@ -11343,7 +11334,7 @@
         <v>16.113631331442001</v>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A129" s="4">
         <v>127</v>
       </c>
@@ -11425,7 +11416,7 @@
         <v>16.120742708005</v>
       </c>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A130" s="4">
         <v>128</v>
       </c>
@@ -11507,7 +11498,7 @@
         <v>16.6599037100797</v>
       </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A131" s="4">
         <v>129</v>
       </c>
@@ -11589,7 +11580,7 @@
         <v>16.705822336562999</v>
       </c>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A132" s="4">
         <v>130</v>
       </c>
@@ -11671,7 +11662,7 @@
         <v>16.7628409089901</v>
       </c>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A133" s="4">
         <v>131</v>
       </c>
@@ -11753,7 +11744,7 @@
         <v>16.150396947228401</v>
       </c>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A134" s="4">
         <v>132</v>
       </c>
@@ -11835,7 +11826,7 @@
         <v>15.3720936341465</v>
       </c>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A135" s="4">
         <v>133</v>
       </c>
@@ -11917,7 +11908,7 @@
         <v>15.207804271541301</v>
       </c>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A136" s="4">
         <v>134</v>
       </c>
@@ -11999,7 +11990,7 @@
         <v>14.607823509938299</v>
       </c>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A137" s="4">
         <v>135</v>
       </c>
@@ -12081,7 +12072,7 @@
         <v>13.6711197999911</v>
       </c>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A138" s="4">
         <v>136</v>
       </c>
@@ -12163,7 +12154,7 @@
         <v>13.937102595633201</v>
       </c>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A139" s="4">
         <v>137</v>
       </c>
@@ -12245,7 +12236,7 @@
         <v>14.305698275808799</v>
       </c>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A140" s="4">
         <v>138</v>
       </c>
@@ -12327,7 +12318,7 @@
         <v>14.243953693353401</v>
       </c>
     </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A141" s="4">
         <v>139</v>
       </c>
@@ -12409,7 +12400,7 @@
         <v>14.366568041736301</v>
       </c>
     </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A142" s="4">
         <v>140</v>
       </c>
@@ -12491,7 +12482,7 @@
         <v>15.1203531340515</v>
       </c>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A143" s="4">
         <v>141</v>
       </c>
@@ -12573,7 +12564,7 @@
         <v>15.691984664705901</v>
       </c>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A144" s="4">
         <v>142</v>
       </c>
@@ -12655,7 +12646,7 @@
         <v>15.3449938541245</v>
       </c>
     </row>
-    <row r="145" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A145" s="4">
         <v>143</v>
       </c>
@@ -12737,7 +12728,7 @@
         <v>15.285300670218</v>
       </c>
     </row>
-    <row r="146" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A146" s="4">
         <v>144</v>
       </c>
@@ -12819,7 +12810,7 @@
         <v>14.727913284457699</v>
       </c>
     </row>
-    <row r="147" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A147" s="4">
         <v>145</v>
       </c>
@@ -12901,7 +12892,7 @@
         <v>14.090988831051201</v>
       </c>
     </row>
-    <row r="148" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A148" s="4">
         <v>146</v>
       </c>
@@ -12983,7 +12974,7 @@
         <v>13.561939402961</v>
       </c>
     </row>
-    <row r="149" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A149" s="4">
         <v>147</v>
       </c>
@@ -13065,7 +13056,7 @@
         <v>13.070679219734499</v>
       </c>
     </row>
-    <row r="150" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A150" s="4">
         <v>148</v>
       </c>
@@ -13147,7 +13138,7 @@
         <v>12.5772595112294</v>
       </c>
     </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A151" s="4">
         <v>149</v>
       </c>
@@ -13229,7 +13220,7 @@
         <v>12.5596040027716</v>
       </c>
     </row>
-    <row r="152" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A152" s="4">
         <v>150</v>
       </c>
@@ -13311,7 +13302,7 @@
         <v>13.110921462571101</v>
       </c>
     </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A153" s="4">
         <v>151</v>
       </c>
@@ -13393,7 +13384,7 @@
         <v>13.062343953195899</v>
       </c>
     </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A154" s="4">
         <v>152</v>
       </c>
@@ -13475,7 +13466,7 @@
         <v>13.252946001101799</v>
       </c>
     </row>
-    <row r="155" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A155" s="4">
         <v>153</v>
       </c>
@@ -13557,7 +13548,7 @@
         <v>13.692593498654</v>
       </c>
     </row>
-    <row r="156" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A156" s="4">
         <v>154</v>
       </c>
@@ -13639,7 +13630,7 @@
         <v>13.699636441906801</v>
       </c>
     </row>
-    <row r="157" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A157" s="4">
         <v>155</v>
       </c>
@@ -13721,7 +13712,7 @@
         <v>13.1356829936324</v>
       </c>
     </row>
-    <row r="158" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A158" s="4">
         <v>156</v>
       </c>
@@ -13803,7 +13794,7 @@
         <v>12.8108158536141</v>
       </c>
     </row>
-    <row r="159" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A159" s="4">
         <v>157</v>
       </c>
@@ -13885,7 +13876,7 @@
         <v>12.816410100620899</v>
       </c>
     </row>
-    <row r="160" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A160" s="4">
         <v>158</v>
       </c>
@@ -13967,7 +13958,7 @@
         <v>13.044485021236101</v>
       </c>
     </row>
-    <row r="161" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A161" s="4">
         <v>159</v>
       </c>
@@ -14049,7 +14040,7 @@
         <v>13.1763539087168</v>
       </c>
     </row>
-    <row r="162" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A162" s="4">
         <v>160</v>
       </c>
@@ -14131,7 +14122,7 @@
         <v>12.479310573888</v>
       </c>
     </row>
-    <row r="163" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A163" s="4">
         <v>161</v>
       </c>
@@ -14213,7 +14204,7 @@
         <v>12.0434436761443</v>
       </c>
     </row>
-    <row r="164" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A164" s="4">
         <v>162</v>
       </c>
@@ -14295,7 +14286,7 @@
         <v>11.7950640075442</v>
       </c>
     </row>
-    <row r="165" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A165" s="4">
         <v>163</v>
       </c>
@@ -14377,7 +14368,7 @@
         <v>11.8679599910823</v>
       </c>
     </row>
-    <row r="166" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A166" s="4">
         <v>164</v>
       </c>
@@ -14459,7 +14450,7 @@
         <v>11.5901761420778</v>
       </c>
     </row>
-    <row r="167" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A167" s="4">
         <v>165</v>
       </c>
@@ -14541,7 +14532,7 @@
         <v>11.895316982337601</v>
       </c>
     </row>
-    <row r="168" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A168" s="4">
         <v>166</v>
       </c>
@@ -14623,7 +14614,7 @@
         <v>11.7665845155101</v>
       </c>
     </row>
-    <row r="169" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A169" s="4">
         <v>167</v>
       </c>
@@ -14705,7 +14696,7 @@
         <v>11.453332262058799</v>
       </c>
     </row>
-    <row r="170" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A170" s="4">
         <v>168</v>
       </c>
@@ -14787,7 +14778,7 @@
         <v>11.386578842492</v>
       </c>
     </row>
-    <row r="171" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A171" s="4">
         <v>169</v>
       </c>
@@ -14869,7 +14860,7 @@
         <v>11.3865920698675</v>
       </c>
     </row>
-    <row r="172" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A172" s="4">
         <v>170</v>
       </c>
@@ -14951,7 +14942,7 @@
         <v>11.530429165428901</v>
       </c>
     </row>
-    <row r="173" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A173" s="4">
         <v>171</v>
       </c>
@@ -15033,7 +15024,7 @@
         <v>11.8785112450217</v>
       </c>
     </row>
-    <row r="174" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A174" s="4">
         <v>172</v>
       </c>
@@ -15115,7 +15106,7 @@
         <v>12.316903208731601</v>
       </c>
     </row>
-    <row r="175" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A175" s="4">
         <v>173</v>
       </c>
@@ -15197,7 +15188,7 @@
         <v>11.879291358187199</v>
       </c>
     </row>
-    <row r="176" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A176" s="4">
         <v>174</v>
       </c>
@@ -15279,7 +15270,7 @@
         <v>11.6775344168566</v>
       </c>
     </row>
-    <row r="177" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A177" s="4">
         <v>175</v>
       </c>
@@ -15361,7 +15352,7 @@
         <v>11.642109123715301</v>
       </c>
     </row>
-    <row r="178" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A178" s="4">
         <v>176</v>
       </c>
@@ -15443,7 +15434,7 @@
         <v>11.498276887877999</v>
       </c>
     </row>
-    <row r="179" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A179" s="4">
         <v>177</v>
       </c>
@@ -15525,7 +15516,7 @@
         <v>11.5180480427939</v>
       </c>
     </row>
-    <row r="180" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A180" s="4">
         <v>178</v>
       </c>
@@ -15607,7 +15598,7 @@
         <v>12.1146615703083</v>
       </c>
     </row>
-    <row r="181" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A181" s="4">
         <v>179</v>
       </c>
@@ -15689,7 +15680,7 @@
         <v>12.2565823130744</v>
       </c>
     </row>
-    <row r="182" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A182" s="4">
         <v>180</v>
       </c>
@@ -15771,7 +15762,7 @@
         <v>12.2678793832705</v>
       </c>
     </row>
-    <row r="183" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A183" s="4">
         <v>181</v>
       </c>
@@ -15853,7 +15844,7 @@
         <v>12.4294502367413</v>
       </c>
     </row>
-    <row r="184" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A184" s="4">
         <v>182</v>
       </c>
@@ -15935,7 +15926,7 @@
         <v>12.361304498200401</v>
       </c>
     </row>
-    <row r="185" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A185" s="4">
         <v>183</v>
       </c>
@@ -16017,7 +16008,7 @@
         <v>11.866143483161499</v>
       </c>
     </row>
-    <row r="186" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A186" s="4">
         <v>184</v>
       </c>
@@ -16099,7 +16090,7 @@
         <v>11.467767805282801</v>
       </c>
     </row>
-    <row r="187" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A187" s="4">
         <v>185</v>
       </c>
@@ -16181,7 +16172,7 @@
         <v>11.445273740109201</v>
       </c>
     </row>
-    <row r="188" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A188" s="4">
         <v>186</v>
       </c>
@@ -16263,7 +16254,7 @@
         <v>11.3991893073767</v>
       </c>
     </row>
-    <row r="189" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A189" s="4">
         <v>187</v>
       </c>
@@ -16345,7 +16336,7 @@
         <v>11.8936194473648</v>
       </c>
     </row>
-    <row r="190" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A190" s="4">
         <v>188</v>
       </c>
@@ -16427,7 +16418,7 @@
         <v>12.7062609107585</v>
       </c>
     </row>
-    <row r="191" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A191" s="4">
         <v>189</v>
       </c>
@@ -16509,7 +16500,7 @@
         <v>13.6572585725811</v>
       </c>
     </row>
-    <row r="192" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A192" s="4">
         <v>190</v>
       </c>
@@ -16591,7 +16582,7 @@
         <v>14.747016123276699</v>
       </c>
     </row>
-    <row r="193" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A193" s="4">
         <v>191</v>
       </c>
@@ -16673,7 +16664,7 @@
         <v>16.282048374839999</v>
       </c>
     </row>
-    <row r="194" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A194" s="4">
         <v>192</v>
       </c>
@@ -16755,7 +16746,7 @@
         <v>17.712003983233199</v>
       </c>
     </row>
-    <row r="195" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A195" s="4">
         <v>193</v>
       </c>
@@ -16837,7 +16828,7 @@
         <v>18.5918000980394</v>
       </c>
     </row>
-    <row r="196" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A196" s="4">
         <v>194</v>
       </c>
@@ -16919,7 +16910,7 @@
         <v>19.498445742313798</v>
       </c>
     </row>
-    <row r="197" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A197" s="4">
         <v>195</v>
       </c>
@@ -17001,7 +16992,7 @@
         <v>20.2589605402109</v>
       </c>
     </row>
-    <row r="198" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A198" s="4">
         <v>196</v>
       </c>
@@ -17083,7 +17074,7 @@
         <v>20.544887992854999</v>
       </c>
     </row>
-    <row r="199" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A199" s="4">
         <v>197</v>
       </c>
@@ -17165,7 +17156,7 @@
         <v>20.932015121038699</v>
       </c>
     </row>
-    <row r="200" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A200" s="4">
         <v>198</v>
       </c>
@@ -17247,7 +17238,7 @@
         <v>21.681003499998699</v>
       </c>
     </row>
-    <row r="201" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A201" s="4">
         <v>199</v>
       </c>
@@ -17329,7 +17320,7 @@
         <v>22.379617101271698</v>
       </c>
     </row>
-    <row r="202" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A202" s="4">
         <v>200</v>
       </c>
@@ -17411,7 +17402,7 @@
         <v>23.488704368278199</v>
       </c>
     </row>
-    <row r="203" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A203" s="4">
         <v>201</v>
       </c>
@@ -17493,7 +17484,7 @@
         <v>23.8833827363759</v>
       </c>
     </row>
-    <row r="204" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A204" s="4">
         <v>202</v>
       </c>
@@ -17575,7 +17566,7 @@
         <v>24.870522999988498</v>
       </c>
     </row>
-    <row r="205" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A205" s="4">
         <v>203</v>
       </c>
@@ -17657,7 +17648,7 @@
         <v>26.040624648346299</v>
       </c>
     </row>
-    <row r="206" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A206" s="4">
         <v>204</v>
       </c>
@@ -17739,7 +17730,7 @@
         <v>27.419787398359698</v>
       </c>
     </row>
-    <row r="207" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A207" s="4">
         <v>205</v>
       </c>
@@ -17821,7 +17812,7 @@
         <v>27.407198372818101</v>
       </c>
     </row>
-    <row r="208" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A208" s="4">
         <v>206</v>
       </c>
@@ -17903,7 +17894,7 @@
         <v>27.260156916497198</v>
       </c>
     </row>
-    <row r="209" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A209" s="4">
         <v>207</v>
       </c>
@@ -17985,7 +17976,7 @@
         <v>27.811560559992301</v>
       </c>
     </row>
-    <row r="210" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A210" s="4">
         <v>208</v>
       </c>
@@ -18067,7 +18058,7 @@
         <v>28.323578228952101</v>
       </c>
     </row>
-    <row r="211" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A211" s="4">
         <v>209</v>
       </c>
@@ -18149,7 +18140,7 @@
         <v>28.810641176833901</v>
       </c>
     </row>
-    <row r="212" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A212" s="4">
         <v>210</v>
       </c>
@@ -18231,7 +18222,7 @@
         <v>29.654156738617399</v>
       </c>
     </row>
-    <row r="213" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A213" s="4">
         <v>211</v>
       </c>
@@ -18313,7 +18304,7 @@
         <v>30.012186955780201</v>
       </c>
     </row>
-    <row r="214" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A214" s="4">
         <v>212</v>
       </c>
@@ -18395,7 +18386,7 @@
         <v>30.6023842791951</v>
       </c>
     </row>
-    <row r="215" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A215" s="4">
         <v>213</v>
       </c>
@@ -18477,7 +18468,7 @@
         <v>31.4350163904464</v>
       </c>
     </row>
-    <row r="216" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A216" s="4">
         <v>214</v>
       </c>
@@ -18559,7 +18550,7 @@
         <v>31.3571049186111</v>
       </c>
     </row>
-    <row r="217" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A217" s="4">
         <v>215</v>
       </c>
@@ -18641,7 +18632,7 @@
         <v>31.7406383790298</v>
       </c>
     </row>
-    <row r="218" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A218" s="4">
         <v>216</v>
       </c>
@@ -18723,7 +18714,7 @@
         <v>31.238266851310399</v>
       </c>
     </row>
-    <row r="219" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A219" s="4">
         <v>217</v>
       </c>
@@ -18805,7 +18796,7 @@
         <v>30.771779004142399</v>
       </c>
     </row>
-    <row r="220" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A220" s="4">
         <v>218</v>
       </c>
@@ -18887,7 +18878,7 @@
         <v>29.168230146264602</v>
       </c>
     </row>
-    <row r="221" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A221" s="4">
         <v>219</v>
       </c>
@@ -18969,7 +18960,7 @@
         <v>27.3320785577477</v>
       </c>
     </row>
-    <row r="222" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A222" s="4">
         <v>220</v>
       </c>
@@ -19051,7 +19042,7 @@
         <v>26.600198382884098</v>
       </c>
     </row>
-    <row r="223" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A223" s="4">
         <v>221</v>
       </c>
@@ -19133,7 +19124,7 @@
         <v>25.899312218927399</v>
       </c>
     </row>
-    <row r="224" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A224" s="4">
         <v>222</v>
       </c>
@@ -19215,7 +19206,7 @@
         <v>25.248489352396099</v>
       </c>
     </row>
-    <row r="225" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A225" s="4">
         <v>223</v>
       </c>
@@ -19297,7 +19288,7 @@
         <v>24.975190286153602</v>
       </c>
     </row>
-    <row r="226" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A226" s="4">
         <v>224</v>
       </c>
@@ -19379,7 +19370,7 @@
         <v>24.797327877659001</v>
       </c>
     </row>
-    <row r="227" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A227" s="4">
         <v>225</v>
       </c>
@@ -19461,7 +19452,7 @@
         <v>24.886786227867599</v>
       </c>
     </row>
-    <row r="228" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A228" s="4">
         <v>226</v>
       </c>
@@ -19543,7 +19534,7 @@
         <v>25.231215737617799</v>
       </c>
     </row>
-    <row r="229" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A229" s="4">
         <v>227</v>
       </c>
@@ -19625,7 +19616,7 @@
         <v>25.743601967571902</v>
       </c>
     </row>
-    <row r="230" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A230" s="4">
         <v>228</v>
       </c>
@@ -19707,7 +19698,7 @@
         <v>26.763867884306698</v>
       </c>
     </row>
-    <row r="231" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A231" s="4">
         <v>229</v>
       </c>
@@ -19789,7 +19780,7 @@
         <v>26.889232646338399</v>
       </c>
     </row>
-    <row r="232" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A232" s="4">
         <v>230</v>
       </c>
@@ -19871,7 +19862,7 @@
         <v>27.378564049755699</v>
       </c>
     </row>
-    <row r="233" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A233" s="4">
         <v>231</v>
       </c>
@@ -19953,7 +19944,7 @@
         <v>26.722578457910199</v>
       </c>
     </row>
-    <row r="234" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A234" s="4">
         <v>232</v>
       </c>
@@ -20035,7 +20026,7 @@
         <v>26.0433872363791</v>
       </c>
     </row>
-    <row r="235" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A235" s="4">
         <v>233</v>
       </c>
@@ -20117,7 +20108,7 @@
         <v>25.432565694878299</v>
       </c>
     </row>
-    <row r="236" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A236" s="4">
         <v>234</v>
       </c>
@@ -20199,7 +20190,7 @@
         <v>24.736998515986201</v>
       </c>
     </row>
-    <row r="237" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A237" s="4">
         <v>235</v>
       </c>
@@ -20281,7 +20272,7 @@
         <v>24.240650205704</v>
       </c>
     </row>
-    <row r="238" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A238" s="4">
         <v>236</v>
       </c>
@@ -20363,7 +20354,7 @@
         <v>23.9990279894261</v>
       </c>
     </row>
-    <row r="239" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A239" s="4">
         <v>237</v>
       </c>
@@ -20445,7 +20436,7 @@
         <v>24.503548672513901</v>
       </c>
     </row>
-    <row r="240" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A240" s="4">
         <v>238</v>
       </c>
@@ -20527,7 +20518,7 @@
         <v>25.134537340839</v>
       </c>
     </row>
-    <row r="241" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A241" s="4">
         <v>239</v>
       </c>
@@ -20609,7 +20600,7 @@
         <v>25.865718685452102</v>
       </c>
     </row>
-    <row r="242" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A242" s="4">
         <v>240</v>
       </c>
@@ -20691,7 +20682,7 @@
         <v>26.2121296786252</v>
       </c>
     </row>
-    <row r="243" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A243" s="4">
         <v>241</v>
       </c>
@@ -20773,7 +20764,7 @@
         <v>27.306221620894199</v>
       </c>
     </row>
-    <row r="244" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A244" s="4">
         <v>242</v>
       </c>
@@ -20855,7 +20846,7 @@
         <v>28.7289945657628</v>
       </c>
     </row>
-    <row r="245" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A245" s="4">
         <v>243</v>
       </c>
@@ -20937,7 +20928,7 @@
         <v>30.081878929691499</v>
       </c>
     </row>
-    <row r="246" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A246" s="4">
         <v>244</v>
       </c>
@@ -21019,7 +21010,7 @@
         <v>29.953416350638701</v>
       </c>
     </row>
-    <row r="247" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A247" s="4">
         <v>245</v>
       </c>
@@ -21101,7 +21092,7 @@
         <v>30.122000749080701</v>
       </c>
     </row>
-    <row r="248" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A248" s="4">
         <v>246</v>
       </c>
@@ -21183,7 +21174,7 @@
         <v>29.764326961141901</v>
       </c>
     </row>
-    <row r="249" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A249" s="4">
         <v>247</v>
       </c>
@@ -21265,7 +21256,7 @@
         <v>29.316410221164901</v>
       </c>
     </row>
-    <row r="250" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A250" s="4">
         <v>248</v>
       </c>
@@ -21313,7 +21304,7 @@
         <f>100*testdata[[#This Row],[-DM14]]/testdata[[#This Row],[TR14]]</f>
         <v>18.247083794191962</v>
       </c>
-      <c r="N250" s="6">
+      <c r="N250" s="11">
         <f>100*ABS(testdata[[#This Row],[+DI14]]-testdata[[#This Row],[-DI14]])/(testdata[[#This Row],[+DI14]]+testdata[[#This Row],[-DI14]])</f>
         <v>27.825450922906132</v>
       </c>
@@ -21347,7 +21338,7 @@
         <v>29.125166308423101</v>
       </c>
     </row>
-    <row r="251" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A251" s="4">
         <v>249</v>
       </c>
@@ -21429,7 +21420,7 @@
         <v>29.2164317967156</v>
       </c>
     </row>
-    <row r="252" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A252" s="4">
         <v>250</v>
       </c>
@@ -21511,7 +21502,7 @@
         <v>29.079359374489599</v>
       </c>
     </row>
-    <row r="253" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A253" s="4">
         <v>251</v>
       </c>
@@ -21593,7 +21584,7 @@
         <v>29.1949732270187</v>
       </c>
     </row>
-    <row r="254" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A254" s="4">
         <v>252</v>
       </c>
@@ -21675,7 +21666,7 @@
         <v>29.833025880740301</v>
       </c>
     </row>
-    <row r="255" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A255" s="4">
         <v>253</v>
       </c>
@@ -21757,7 +21748,7 @@
         <v>30.321430073304999</v>
       </c>
     </row>
-    <row r="256" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A256" s="4">
         <v>254</v>
       </c>
@@ -21839,7 +21830,7 @@
         <v>31.241288391566101</v>
       </c>
     </row>
-    <row r="257" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A257" s="4">
         <v>255</v>
       </c>
@@ -21921,7 +21912,7 @@
         <v>32.442144175962397</v>
       </c>
     </row>
-    <row r="258" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A258" s="4">
         <v>256</v>
       </c>
@@ -22003,7 +21994,7 @@
         <v>33.380723590489403</v>
       </c>
     </row>
-    <row r="259" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A259" s="4">
         <v>257</v>
       </c>
@@ -22085,7 +22076,7 @@
         <v>33.576693497222898</v>
       </c>
     </row>
-    <row r="260" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A260" s="4">
         <v>258</v>
       </c>
@@ -22167,7 +22158,7 @@
         <v>34.039171782289998</v>
       </c>
     </row>
-    <row r="261" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A261" s="4">
         <v>259</v>
       </c>
@@ -22249,7 +22240,7 @@
         <v>34.5633153964095</v>
       </c>
     </row>
-    <row r="262" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A262" s="4">
         <v>260</v>
       </c>
@@ -22331,7 +22322,7 @@
         <v>35.243272783614103</v>
       </c>
     </row>
-    <row r="263" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A263" s="4">
         <v>261</v>
       </c>
@@ -22413,7 +22404,7 @@
         <v>35.9498050617091</v>
       </c>
     </row>
-    <row r="264" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A264" s="4">
         <v>262</v>
       </c>
@@ -22495,7 +22486,7 @@
         <v>36.655447226794401</v>
       </c>
     </row>
-    <row r="265" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A265" s="4">
         <v>263</v>
       </c>
@@ -22577,7 +22568,7 @@
         <v>36.978448067860199</v>
       </c>
     </row>
-    <row r="266" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A266" s="4">
         <v>264</v>
       </c>
@@ -22659,7 +22650,7 @@
         <v>37.571222731222598</v>
       </c>
     </row>
-    <row r="267" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A267" s="4">
         <v>265</v>
       </c>
@@ -22741,7 +22732,7 @@
         <v>38.683797841457</v>
       </c>
     </row>
-    <row r="268" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A268" s="4">
         <v>266</v>
       </c>
@@ -22823,7 +22814,7 @@
         <v>40.108469578976297</v>
       </c>
     </row>
-    <row r="269" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A269" s="4">
         <v>267</v>
       </c>
@@ -22905,7 +22896,7 @@
         <v>41.669773300721502</v>
       </c>
     </row>
-    <row r="270" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A270" s="4">
         <v>268</v>
       </c>
@@ -22987,7 +22978,7 @@
         <v>43.355401407904203</v>
       </c>
     </row>
-    <row r="271" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A271" s="4">
         <v>269</v>
       </c>
@@ -23069,7 +23060,7 @@
         <v>45.0853097599989</v>
       </c>
     </row>
-    <row r="272" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A272" s="4">
         <v>270</v>
       </c>
@@ -23151,7 +23142,7 @@
         <v>44.8302113134135</v>
       </c>
     </row>
-    <row r="273" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A273" s="4">
         <v>271</v>
       </c>
@@ -23233,7 +23224,7 @@
         <v>44.682997203934796</v>
       </c>
     </row>
-    <row r="274" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A274" s="4">
         <v>272</v>
       </c>
@@ -23315,7 +23306,7 @@
         <v>44.800202646040198</v>
       </c>
     </row>
-    <row r="275" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A275" s="4">
         <v>273</v>
       </c>
@@ -23397,7 +23388,7 @@
         <v>43.949283404165698</v>
       </c>
     </row>
-    <row r="276" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A276" s="4">
         <v>274</v>
       </c>
@@ -23479,7 +23470,7 @@
         <v>44.595460482788901</v>
       </c>
     </row>
-    <row r="277" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A277" s="4">
         <v>275</v>
       </c>
@@ -23561,7 +23552,7 @@
         <v>45.489532518218297</v>
       </c>
     </row>
-    <row r="278" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A278" s="4">
         <v>276</v>
       </c>
@@ -23643,7 +23634,7 @@
         <v>45.917445996110096</v>
       </c>
     </row>
-    <row r="279" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A279" s="4">
         <v>277</v>
       </c>
@@ -23725,7 +23716,7 @@
         <v>47.073628957847298</v>
       </c>
     </row>
-    <row r="280" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A280" s="4">
         <v>278</v>
       </c>
@@ -23807,7 +23798,7 @@
         <v>48.402261377820203</v>
       </c>
     </row>
-    <row r="281" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A281" s="4">
         <v>279</v>
       </c>
@@ -23889,7 +23880,7 @@
         <v>49.253150487665899</v>
       </c>
     </row>
-    <row r="282" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A282" s="4">
         <v>280</v>
       </c>
@@ -23971,7 +23962,7 @@
         <v>50.043261803951097</v>
       </c>
     </row>
-    <row r="283" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A283" s="4">
         <v>281</v>
       </c>
@@ -24053,7 +24044,7 @@
         <v>50.482810002419299</v>
       </c>
     </row>
-    <row r="284" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A284" s="4">
         <v>282</v>
       </c>
@@ -24135,7 +24126,7 @@
         <v>50.524515847224599</v>
       </c>
     </row>
-    <row r="285" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A285" s="4">
         <v>283</v>
       </c>
@@ -24217,7 +24208,7 @@
         <v>48.9727311126397</v>
       </c>
     </row>
-    <row r="286" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A286" s="4">
         <v>284</v>
       </c>
@@ -24299,7 +24290,7 @@
         <v>47.489243388807999</v>
       </c>
     </row>
-    <row r="287" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A287" s="4">
         <v>285</v>
       </c>
@@ -24381,7 +24372,7 @@
         <v>45.988055235207099</v>
       </c>
     </row>
-    <row r="288" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A288" s="4">
         <v>286</v>
       </c>
@@ -24463,7 +24454,7 @@
         <v>43.458459724148398</v>
       </c>
     </row>
-    <row r="289" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A289" s="4">
         <v>287</v>
       </c>
@@ -24545,7 +24536,7 @@
         <v>42.336710251636497</v>
       </c>
     </row>
-    <row r="290" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A290" s="4">
         <v>288</v>
       </c>
@@ -24627,7 +24618,7 @@
         <v>41.204624480284501</v>
       </c>
     </row>
-    <row r="291" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A291" s="4">
         <v>289</v>
       </c>
@@ -24709,7 +24700,7 @@
         <v>39.703261507314402</v>
       </c>
     </row>
-    <row r="292" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A292" s="4">
         <v>290</v>
       </c>
@@ -24791,7 +24782,7 @@
         <v>39.186372254460899</v>
       </c>
     </row>
-    <row r="293" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A293" s="4">
         <v>291</v>
       </c>
@@ -24873,7 +24864,7 @@
         <v>39.364514982524398</v>
       </c>
     </row>
-    <row r="294" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A294" s="4">
         <v>292</v>
       </c>
@@ -24955,7 +24946,7 @@
         <v>39.162926652029299</v>
       </c>
     </row>
-    <row r="295" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A295" s="4">
         <v>293</v>
       </c>
@@ -25037,7 +25028,7 @@
         <v>38.5659328083131</v>
       </c>
     </row>
-    <row r="296" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A296" s="4">
         <v>294</v>
       </c>
@@ -25119,7 +25110,7 @@
         <v>37.502797409335997</v>
       </c>
     </row>
-    <row r="297" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A297" s="4">
         <v>295</v>
       </c>
@@ -25201,7 +25192,7 @@
         <v>36.244865030022403</v>
       </c>
     </row>
-    <row r="298" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A298" s="4">
         <v>296</v>
       </c>
@@ -25283,7 +25274,7 @@
         <v>34.674984555811697</v>
       </c>
     </row>
-    <row r="299" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A299" s="4">
         <v>297</v>
       </c>
@@ -25365,7 +25356,7 @@
         <v>33.072077162676301</v>
       </c>
     </row>
-    <row r="300" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A300" s="4">
         <v>298</v>
       </c>
@@ -25447,7 +25438,7 @@
         <v>31.572873004156001</v>
       </c>
     </row>
-    <row r="301" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A301" s="4">
         <v>299</v>
       </c>
@@ -25529,7 +25520,7 @@
         <v>29.9561712714073</v>
       </c>
     </row>
-    <row r="302" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A302" s="4">
         <v>300</v>
       </c>
@@ -25611,7 +25602,7 @@
         <v>28.400852893868699</v>
       </c>
     </row>
-    <row r="303" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A303" s="4">
         <v>301</v>
       </c>
@@ -25693,7 +25684,7 @@
         <v>26.600677803712301</v>
       </c>
     </row>
-    <row r="304" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A304" s="4">
         <v>302</v>
       </c>
@@ -25775,7 +25766,7 @@
         <v>24.9290866485671</v>
       </c>
     </row>
-    <row r="305" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A305" s="4">
         <v>303</v>
       </c>
@@ -25857,7 +25848,7 @@
         <v>24.330164002215401</v>
       </c>
     </row>
-    <row r="306" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A306" s="4">
         <v>304</v>
       </c>
@@ -25939,7 +25930,7 @@
         <v>24.249288733771099</v>
       </c>
     </row>
-    <row r="307" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A307" s="4">
         <v>305</v>
       </c>
@@ -26021,7 +26012,7 @@
         <v>24.012982288271299</v>
       </c>
     </row>
-    <row r="308" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A308" s="4">
         <v>306</v>
       </c>
@@ -26103,7 +26094,7 @@
         <v>24.021074651591999</v>
       </c>
     </row>
-    <row r="309" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A309" s="4">
         <v>307</v>
       </c>
@@ -26185,7 +26176,7 @@
         <v>24.3361205913288</v>
       </c>
     </row>
-    <row r="310" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A310" s="4">
         <v>308</v>
       </c>
@@ -26267,7 +26258,7 @@
         <v>24.6609309569155</v>
       </c>
     </row>
-    <row r="311" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A311" s="4">
         <v>309</v>
       </c>
@@ -26349,7 +26340,7 @@
         <v>24.609799024355802</v>
       </c>
     </row>
-    <row r="312" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A312" s="4">
         <v>310</v>
       </c>
@@ -26431,7 +26422,7 @@
         <v>24.299107490012901</v>
       </c>
     </row>
-    <row r="313" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A313" s="4">
         <v>311</v>
       </c>
@@ -26513,7 +26504,7 @@
         <v>23.708973109991799</v>
       </c>
     </row>
-    <row r="314" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A314" s="4">
         <v>312</v>
       </c>
@@ -26595,7 +26586,7 @@
         <v>23.320559083278098</v>
       </c>
     </row>
-    <row r="315" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A315" s="4">
         <v>313</v>
       </c>
@@ -26677,7 +26668,7 @@
         <v>23.114949305379099</v>
       </c>
     </row>
-    <row r="316" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A316" s="4">
         <v>314</v>
       </c>
@@ -26759,7 +26750,7 @@
         <v>22.4902681345764</v>
       </c>
     </row>
-    <row r="317" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A317" s="4">
         <v>315</v>
       </c>
@@ -26841,7 +26832,7 @@
         <v>21.5965931053479</v>
       </c>
     </row>
-    <row r="318" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A318" s="4">
         <v>316</v>
       </c>
@@ -26923,7 +26914,7 @@
         <v>21.920946856281098</v>
       </c>
     </row>
-    <row r="319" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A319" s="4">
         <v>317</v>
       </c>
@@ -27005,7 +26996,7 @@
         <v>22.2221324821477</v>
       </c>
     </row>
-    <row r="320" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A320" s="4">
         <v>318</v>
       </c>
@@ -27087,7 +27078,7 @@
         <v>22.075075981773001</v>
       </c>
     </row>
-    <row r="321" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A321" s="4">
         <v>319</v>
       </c>
@@ -27169,7 +27160,7 @@
         <v>22.5758479738234</v>
       </c>
     </row>
-    <row r="322" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A322" s="4">
         <v>320</v>
       </c>
@@ -27251,7 +27242,7 @@
         <v>23.204105080850901</v>
       </c>
     </row>
-    <row r="323" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A323" s="4">
         <v>321</v>
       </c>
@@ -27333,7 +27324,7 @@
         <v>23.831982200405601</v>
       </c>
     </row>
-    <row r="324" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A324" s="4">
         <v>322</v>
       </c>
@@ -27415,7 +27406,7 @@
         <v>24.100669583639199</v>
       </c>
     </row>
-    <row r="325" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A325" s="4">
         <v>323</v>
       </c>
@@ -27497,7 +27488,7 @@
         <v>23.957310799270498</v>
       </c>
     </row>
-    <row r="326" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A326" s="4">
         <v>324</v>
       </c>
@@ -27579,7 +27570,7 @@
         <v>23.347236408235101</v>
       </c>
     </row>
-    <row r="327" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A327" s="4">
         <v>325</v>
       </c>
@@ -27661,7 +27652,7 @@
         <v>23.465210872016701</v>
       </c>
     </row>
-    <row r="328" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A328" s="4">
         <v>326</v>
       </c>
@@ -27743,7 +27734,7 @@
         <v>23.819705472483701</v>
       </c>
     </row>
-    <row r="329" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A329" s="4">
         <v>327</v>
       </c>
@@ -27825,7 +27816,7 @@
         <v>23.716015492394899</v>
       </c>
     </row>
-    <row r="330" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A330" s="4">
         <v>328</v>
       </c>
@@ -27907,7 +27898,7 @@
         <v>23.7268905067628</v>
       </c>
     </row>
-    <row r="331" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A331" s="4">
         <v>329</v>
       </c>
@@ -27989,7 +27980,7 @@
         <v>24.308211406051001</v>
       </c>
     </row>
-    <row r="332" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A332" s="4">
         <v>330</v>
       </c>
@@ -28071,7 +28062,7 @@
         <v>24.296009563747699</v>
       </c>
     </row>
-    <row r="333" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A333" s="4">
         <v>331</v>
       </c>
@@ -28153,7 +28144,7 @@
         <v>24.0975316290112</v>
       </c>
     </row>
-    <row r="334" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A334" s="4">
         <v>332</v>
       </c>
@@ -28235,7 +28226,7 @@
         <v>24.040589746413101</v>
       </c>
     </row>
-    <row r="335" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A335" s="4">
         <v>333</v>
       </c>
@@ -28317,7 +28308,7 @@
         <v>24.040297779885101</v>
       </c>
     </row>
-    <row r="336" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A336" s="4">
         <v>334</v>
       </c>
@@ -28399,7 +28390,7 @@
         <v>24.0358557453396</v>
       </c>
     </row>
-    <row r="337" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A337" s="4">
         <v>335</v>
       </c>
@@ -28481,7 +28472,7 @@
         <v>24.3059452059323</v>
       </c>
     </row>
-    <row r="338" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A338" s="4">
         <v>336</v>
       </c>
@@ -28563,7 +28554,7 @@
         <v>23.5333877332789</v>
       </c>
     </row>
-    <row r="339" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A339" s="4">
         <v>337</v>
       </c>
@@ -28645,7 +28636,7 @@
         <v>22.5567838939</v>
       </c>
     </row>
-    <row r="340" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A340" s="4">
         <v>338</v>
       </c>
@@ -28727,7 +28718,7 @@
         <v>22.037988007839701</v>
       </c>
     </row>
-    <row r="341" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A341" s="4">
         <v>339</v>
       </c>
@@ -28809,7 +28800,7 @@
         <v>21.400084393895899</v>
       </c>
     </row>
-    <row r="342" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A342" s="4">
         <v>340</v>
       </c>
@@ -28891,7 +28882,7 @@
         <v>20.774055296181899</v>
       </c>
     </row>
-    <row r="343" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A343" s="4">
         <v>341</v>
       </c>
@@ -28973,7 +28964,7 @@
         <v>20.713454193698698</v>
       </c>
     </row>
-    <row r="344" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A344" s="4">
         <v>342</v>
       </c>
@@ -29055,7 +29046,7 @@
         <v>20.820641487708102</v>
       </c>
     </row>
-    <row r="345" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A345" s="4">
         <v>343</v>
       </c>
@@ -29137,7 +29128,7 @@
         <v>20.007212094078799</v>
       </c>
     </row>
-    <row r="346" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A346" s="4">
         <v>344</v>
       </c>
@@ -29219,7 +29210,7 @@
         <v>19.400862031148701</v>
       </c>
     </row>
-    <row r="347" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A347" s="4">
         <v>345</v>
       </c>
@@ -29301,7 +29292,7 @@
         <v>19.033849901852602</v>
       </c>
     </row>
-    <row r="348" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A348" s="4">
         <v>346</v>
       </c>
@@ -29383,7 +29374,7 @@
         <v>18.916167065472699</v>
       </c>
     </row>
-    <row r="349" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A349" s="4">
         <v>347</v>
       </c>
@@ -29465,7 +29456,7 @@
         <v>18.9864164410826</v>
       </c>
     </row>
-    <row r="350" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A350" s="4">
         <v>348</v>
       </c>
@@ -29547,7 +29538,7 @@
         <v>19.4721973298854</v>
       </c>
     </row>
-    <row r="351" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A351" s="4">
         <v>349</v>
       </c>
@@ -29629,7 +29620,7 @@
         <v>19.065660266944601</v>
       </c>
     </row>
-    <row r="352" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A352" s="4">
         <v>350</v>
       </c>
@@ -29711,7 +29702,7 @@
         <v>18.450557253607801</v>
       </c>
     </row>
-    <row r="353" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A353" s="4">
         <v>351</v>
       </c>
@@ -29793,7 +29784,7 @@
         <v>17.993188939884899</v>
       </c>
     </row>
-    <row r="354" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A354" s="4">
         <v>352</v>
       </c>
@@ -29875,7 +29866,7 @@
         <v>17.370528133367301</v>
       </c>
     </row>
-    <row r="355" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A355" s="4">
         <v>353</v>
       </c>
@@ -29957,7 +29948,7 @@
         <v>16.361103887229799</v>
       </c>
     </row>
-    <row r="356" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A356" s="4">
         <v>354</v>
       </c>
@@ -30039,7 +30030,7 @@
         <v>15.552843087417999</v>
       </c>
     </row>
-    <row r="357" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A357" s="4">
         <v>355</v>
       </c>
@@ -30121,7 +30112,7 @@
         <v>14.9670865577054</v>
       </c>
     </row>
-    <row r="358" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A358" s="4">
         <v>356</v>
       </c>
@@ -30203,7 +30194,7 @@
         <v>14.2776973816188</v>
       </c>
     </row>
-    <row r="359" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A359" s="4">
         <v>357</v>
       </c>
@@ -30285,7 +30276,7 @@
         <v>13.8608899240038</v>
       </c>
     </row>
-    <row r="360" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A360" s="4">
         <v>358</v>
       </c>
@@ -30367,7 +30358,7 @@
         <v>13.8678426711318</v>
       </c>
     </row>
-    <row r="361" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A361" s="4">
         <v>359</v>
       </c>
@@ -30449,7 +30440,7 @@
         <v>13.9525434693052</v>
       </c>
     </row>
-    <row r="362" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A362" s="4">
         <v>360</v>
       </c>
@@ -30531,7 +30522,7 @@
         <v>14.3228300719055</v>
       </c>
     </row>
-    <row r="363" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A363" s="4">
         <v>361</v>
       </c>
@@ -30613,7 +30604,7 @@
         <v>14.884309733596799</v>
       </c>
     </row>
-    <row r="364" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A364" s="4">
         <v>362</v>
       </c>
@@ -30695,7 +30686,7 @@
         <v>15.1235247980179</v>
       </c>
     </row>
-    <row r="365" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A365" s="4">
         <v>363</v>
       </c>
@@ -30777,7 +30768,7 @@
         <v>15.190511916975399</v>
       </c>
     </row>
-    <row r="366" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A366" s="4">
         <v>364</v>
       </c>
@@ -30859,7 +30850,7 @@
         <v>15.2527142417217</v>
       </c>
     </row>
-    <row r="367" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A367" s="4">
         <v>365</v>
       </c>
@@ -30941,7 +30932,7 @@
         <v>15.064245297757999</v>
       </c>
     </row>
-    <row r="368" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A368" s="4">
         <v>366</v>
       </c>
@@ -31023,7 +31014,7 @@
         <v>14.4087144661494</v>
       </c>
     </row>
-    <row r="369" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A369" s="4">
         <v>367</v>
       </c>
@@ -31105,7 +31096,7 @@
         <v>13.5452486298121</v>
       </c>
     </row>
-    <row r="370" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A370" s="4">
         <v>368</v>
       </c>
@@ -31187,7 +31178,7 @@
         <v>12.9272276871381</v>
       </c>
     </row>
-    <row r="371" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A371" s="4">
         <v>369</v>
       </c>
@@ -31269,7 +31260,7 @@
         <v>12.6547212717257</v>
       </c>
     </row>
-    <row r="372" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A372" s="4">
         <v>370</v>
       </c>
@@ -31351,7 +31342,7 @@
         <v>12.4603744291437</v>
       </c>
     </row>
-    <row r="373" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A373" s="4">
         <v>371</v>
       </c>
@@ -31433,7 +31424,7 @@
         <v>13.563590916138001</v>
       </c>
     </row>
-    <row r="374" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A374" s="4">
         <v>372</v>
       </c>
@@ -31515,7 +31506,7 @@
         <v>14.7019891631258</v>
       </c>
     </row>
-    <row r="375" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A375" s="4">
         <v>373</v>
       </c>
@@ -31597,7 +31588,7 @@
         <v>15.972210649169</v>
       </c>
     </row>
-    <row r="376" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A376" s="4">
         <v>374</v>
       </c>
@@ -31679,7 +31670,7 @@
         <v>17.4146380538457</v>
       </c>
     </row>
-    <row r="377" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A377" s="4">
         <v>375</v>
       </c>
@@ -31761,7 +31752,7 @@
         <v>18.168954250697599</v>
       </c>
     </row>
-    <row r="378" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A378" s="4">
         <v>376</v>
       </c>
@@ -31843,7 +31834,7 @@
         <v>19.023318463398201</v>
       </c>
     </row>
-    <row r="379" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A379" s="4">
         <v>377</v>
       </c>
@@ -31925,7 +31916,7 @@
         <v>19.565028793365201</v>
       </c>
     </row>
-    <row r="380" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A380" s="4">
         <v>378</v>
       </c>
@@ -32007,7 +31998,7 @@
         <v>19.562903121324101</v>
       </c>
     </row>
-    <row r="381" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A381" s="4">
         <v>379</v>
       </c>
@@ -32089,7 +32080,7 @@
         <v>18.794050732586101</v>
       </c>
     </row>
-    <row r="382" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A382" s="4">
         <v>380</v>
       </c>
@@ -32171,7 +32162,7 @@
         <v>17.636341940310299</v>
       </c>
     </row>
-    <row r="383" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A383" s="4">
         <v>381</v>
       </c>
@@ -32253,7 +32244,7 @@
         <v>16.8959692304635</v>
       </c>
     </row>
-    <row r="384" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A384" s="4">
         <v>382</v>
       </c>
@@ -32335,7 +32326,7 @@
         <v>15.9743349349905</v>
       </c>
     </row>
-    <row r="385" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A385" s="4">
         <v>383</v>
       </c>
@@ -32417,7 +32408,7 @@
         <v>15.378211183727</v>
       </c>
     </row>
-    <row r="386" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A386" s="4">
         <v>384</v>
       </c>
@@ -32499,7 +32490,7 @@
         <v>15.8727196009918</v>
       </c>
     </row>
-    <row r="387" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A387" s="4">
         <v>385</v>
       </c>
@@ -32581,7 +32572,7 @@
         <v>16.331905988451901</v>
       </c>
     </row>
-    <row r="388" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A388" s="4">
         <v>386</v>
       </c>
@@ -32663,7 +32654,7 @@
         <v>17.1822329095613</v>
       </c>
     </row>
-    <row r="389" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A389" s="4">
         <v>387</v>
       </c>
@@ -32745,7 +32736,7 @@
         <v>18.110362038823698</v>
       </c>
     </row>
-    <row r="390" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A390" s="4">
         <v>388</v>
       </c>
@@ -32827,7 +32818,7 @@
         <v>18.2596895435288</v>
       </c>
     </row>
-    <row r="391" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A391" s="4">
         <v>389</v>
       </c>
@@ -32909,7 +32900,7 @@
         <v>18.666597694851198</v>
       </c>
     </row>
-    <row r="392" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A392" s="4">
         <v>390</v>
       </c>
@@ -32991,7 +32982,7 @@
         <v>18.6654025041172</v>
       </c>
     </row>
-    <row r="393" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A393" s="4">
         <v>391</v>
       </c>
@@ -33073,7 +33064,7 @@
         <v>19.074902798161101</v>
       </c>
     </row>
-    <row r="394" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A394" s="4">
         <v>392</v>
       </c>
@@ -33155,7 +33146,7 @@
         <v>19.123796163093498</v>
       </c>
     </row>
-    <row r="395" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A395" s="4">
         <v>393</v>
       </c>
@@ -33237,7 +33228,7 @@
         <v>19.009303941781699</v>
       </c>
     </row>
-    <row r="396" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A396" s="4">
         <v>394</v>
       </c>
@@ -33319,7 +33310,7 @@
         <v>18.307842361126099</v>
       </c>
     </row>
-    <row r="397" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A397" s="4">
         <v>395</v>
       </c>
@@ -33401,7 +33392,7 @@
         <v>17.0879358103426</v>
       </c>
     </row>
-    <row r="398" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A398" s="4">
         <v>396</v>
       </c>
@@ -33483,7 +33474,7 @@
         <v>16.290524284807301</v>
       </c>
     </row>
-    <row r="399" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A399" s="4">
         <v>397</v>
       </c>
@@ -33565,7 +33556,7 @@
         <v>15.575556265207601</v>
       </c>
     </row>
-    <row r="400" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A400" s="4">
         <v>398</v>
       </c>
@@ -33647,7 +33638,7 @@
         <v>14.974989311149301</v>
       </c>
     </row>
-    <row r="401" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A401" s="4">
         <v>399</v>
       </c>
@@ -33729,7 +33720,7 @@
         <v>14.592319179051501</v>
       </c>
     </row>
-    <row r="402" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A402" s="4">
         <v>400</v>
       </c>
@@ -33811,7 +33802,7 @@
         <v>14.6044250109464</v>
       </c>
     </row>
-    <row r="403" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A403" s="4">
         <v>401</v>
       </c>
@@ -33893,7 +33884,7 @@
         <v>14.670969027999099</v>
       </c>
     </row>
-    <row r="404" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A404" s="4">
         <v>402</v>
       </c>
@@ -33975,7 +33966,7 @@
         <v>14.641936624316999</v>
       </c>
     </row>
-    <row r="405" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A405" s="4">
         <v>403</v>
       </c>
@@ -34057,7 +34048,7 @@
         <v>14.501903250587301</v>
       </c>
     </row>
-    <row r="406" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A406" s="4">
         <v>404</v>
       </c>
@@ -34139,7 +34130,7 @@
         <v>14.408782776300701</v>
       </c>
     </row>
-    <row r="407" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A407" s="4">
         <v>405</v>
       </c>
@@ -34221,7 +34212,7 @@
         <v>14.787537026659299</v>
       </c>
     </row>
-    <row r="408" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A408" s="4">
         <v>406</v>
       </c>
@@ -34303,7 +34294,7 @@
         <v>15.136210145418</v>
       </c>
     </row>
-    <row r="409" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A409" s="4">
         <v>407</v>
       </c>
@@ -34385,7 +34376,7 @@
         <v>15.197387871054801</v>
       </c>
     </row>
-    <row r="410" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A410" s="4">
         <v>408</v>
       </c>
@@ -34467,7 +34458,7 @@
         <v>14.3193647860939</v>
       </c>
     </row>
-    <row r="411" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A411" s="4">
         <v>409</v>
       </c>
@@ -34549,7 +34540,7 @@
         <v>13.455772188056899</v>
       </c>
     </row>
-    <row r="412" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A412" s="4">
         <v>410</v>
       </c>
@@ -34631,7 +34622,7 @@
         <v>12.6872116218054</v>
       </c>
     </row>
-    <row r="413" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A413" s="4">
         <v>411</v>
       </c>
@@ -34713,7 +34704,7 @@
         <v>12.3476066811418</v>
       </c>
     </row>
-    <row r="414" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A414" s="4">
         <v>412</v>
       </c>
@@ -34795,7 +34786,7 @@
         <v>11.958458425863901</v>
       </c>
     </row>
-    <row r="415" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A415" s="4">
         <v>413</v>
       </c>
@@ -34877,7 +34868,7 @@
         <v>11.9543942276407</v>
       </c>
     </row>
-    <row r="416" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A416" s="4">
         <v>414</v>
       </c>
@@ -34959,7 +34950,7 @@
         <v>12.346677481393</v>
       </c>
     </row>
-    <row r="417" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A417" s="4">
         <v>415</v>
       </c>
@@ -35041,7 +35032,7 @@
         <v>13.0859098694095</v>
       </c>
     </row>
-    <row r="418" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A418" s="4">
         <v>416</v>
       </c>
@@ -35123,7 +35114,7 @@
         <v>13.880547133235901</v>
       </c>
     </row>
-    <row r="419" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A419" s="4">
         <v>417</v>
       </c>
@@ -35205,7 +35196,7 @@
         <v>14.4148382275316</v>
       </c>
     </row>
-    <row r="420" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A420" s="4">
         <v>418</v>
       </c>
@@ -35287,7 +35278,7 @@
         <v>14.957807606987</v>
       </c>
     </row>
-    <row r="421" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A421" s="4">
         <v>419</v>
       </c>
@@ -35369,7 +35360,7 @@
         <v>15.3296561037263</v>
       </c>
     </row>
-    <row r="422" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A422" s="4">
         <v>420</v>
       </c>
@@ -35451,7 +35442,7 @@
         <v>15.968613297333301</v>
       </c>
     </row>
-    <row r="423" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A423" s="4">
         <v>421</v>
       </c>
@@ -35533,7 +35524,7 @@
         <v>15.587223497216399</v>
       </c>
     </row>
-    <row r="424" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A424" s="4">
         <v>422</v>
       </c>
@@ -35615,7 +35606,7 @@
         <v>14.807751837768199</v>
       </c>
     </row>
-    <row r="425" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A425" s="4">
         <v>423</v>
       </c>
@@ -35697,7 +35688,7 @@
         <v>14.0858205828425</v>
       </c>
     </row>
-    <row r="426" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A426" s="4">
         <v>424</v>
       </c>
@@ -35779,7 +35770,7 @@
         <v>13.8267905444765</v>
       </c>
     </row>
-    <row r="427" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A427" s="4">
         <v>425</v>
       </c>
@@ -35861,7 +35852,7 @@
         <v>13.239849190144</v>
       </c>
     </row>
-    <row r="428" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A428" s="4">
         <v>426</v>
       </c>
@@ -35943,7 +35934,7 @@
         <v>12.8184044512486</v>
       </c>
     </row>
-    <row r="429" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A429" s="4">
         <v>427</v>
       </c>
@@ -36025,7 +36016,7 @@
         <v>12.9848088164429</v>
       </c>
     </row>
-    <row r="430" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A430" s="4">
         <v>428</v>
       </c>
@@ -36107,7 +36098,7 @@
         <v>13.6733974281626</v>
       </c>
     </row>
-    <row r="431" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A431" s="4">
         <v>429</v>
       </c>
@@ -36189,7 +36180,7 @@
         <v>14.0396838581923</v>
       </c>
     </row>
-    <row r="432" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A432" s="4">
         <v>430</v>
       </c>
@@ -36271,7 +36262,7 @@
         <v>14.830533018637199</v>
       </c>
     </row>
-    <row r="433" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A433" s="4">
         <v>431</v>
       </c>
@@ -36353,7 +36344,7 @@
         <v>15.504727933627199</v>
       </c>
     </row>
-    <row r="434" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A434" s="4">
         <v>432</v>
       </c>
@@ -36435,7 +36426,7 @@
         <v>16.6004438243355</v>
       </c>
     </row>
-    <row r="435" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A435" s="4">
         <v>433</v>
       </c>
@@ -36517,7 +36508,7 @@
         <v>17.520967675199099</v>
       </c>
     </row>
-    <row r="436" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A436" s="4">
         <v>434</v>
       </c>
@@ -36599,7 +36590,7 @@
         <v>17.5201980007906</v>
       </c>
     </row>
-    <row r="437" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A437" s="4">
         <v>435</v>
       </c>
@@ -36681,7 +36672,7 @@
         <v>17.258230265366201</v>
       </c>
     </row>
-    <row r="438" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A438" s="4">
         <v>436</v>
       </c>
@@ -36763,7 +36754,7 @@
         <v>16.526766103900702</v>
       </c>
     </row>
-    <row r="439" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A439" s="4">
         <v>437</v>
       </c>
@@ -36845,7 +36836,7 @@
         <v>15.948157559890999</v>
       </c>
     </row>
-    <row r="440" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A440" s="4">
         <v>438</v>
       </c>
@@ -36927,7 +36918,7 @@
         <v>15.0443602217851</v>
       </c>
     </row>
-    <row r="441" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A441" s="4">
         <v>439</v>
       </c>
@@ -37009,7 +37000,7 @@
         <v>14.787644812962601</v>
       </c>
     </row>
-    <row r="442" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A442" s="4">
         <v>440</v>
       </c>
@@ -37091,7 +37082,7 @@
         <v>14.929267156716</v>
       </c>
     </row>
-    <row r="443" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A443" s="4">
         <v>441</v>
       </c>
@@ -37173,7 +37164,7 @@
         <v>15.363294955236601</v>
       </c>
     </row>
-    <row r="444" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A444" s="4">
         <v>442</v>
       </c>
@@ -37255,7 +37246,7 @@
         <v>14.755581750279401</v>
       </c>
     </row>
-    <row r="445" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A445" s="4">
         <v>443</v>
       </c>
@@ -37337,7 +37328,7 @@
         <v>14.7586480006429</v>
       </c>
     </row>
-    <row r="446" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A446" s="4">
         <v>444</v>
       </c>
@@ -37419,7 +37410,7 @@
         <v>14.951896562116101</v>
       </c>
     </row>
-    <row r="447" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A447" s="4">
         <v>445</v>
       </c>
@@ -37501,7 +37492,7 @@
         <v>15.5170034839955</v>
       </c>
     </row>
-    <row r="448" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A448" s="4">
         <v>446</v>
       </c>
@@ -37583,7 +37574,7 @@
         <v>17.431205146225601</v>
       </c>
     </row>
-    <row r="449" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A449" s="4">
         <v>447</v>
       </c>
@@ -37665,7 +37656,7 @@
         <v>19.1206474373075</v>
       </c>
     </row>
-    <row r="450" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A450" s="4">
         <v>448</v>
       </c>
@@ -37747,7 +37738,7 @@
         <v>20.7295214615167</v>
       </c>
     </row>
-    <row r="451" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A451" s="4">
         <v>449</v>
       </c>
@@ -37829,7 +37820,7 @@
         <v>21.8309555281553</v>
       </c>
     </row>
-    <row r="452" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A452" s="4">
         <v>450</v>
       </c>
@@ -37911,7 +37902,7 @@
         <v>21.9815681323878</v>
       </c>
     </row>
-    <row r="453" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A453" s="4">
         <v>451</v>
       </c>
@@ -37993,7 +37984,7 @@
         <v>21.994878157898899</v>
       </c>
     </row>
-    <row r="454" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A454" s="4">
         <v>452</v>
       </c>
@@ -38075,7 +38066,7 @@
         <v>22.736988437650801</v>
       </c>
     </row>
-    <row r="455" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A455" s="4">
         <v>453</v>
       </c>
@@ -38157,7 +38148,7 @@
         <v>23.426090840277599</v>
       </c>
     </row>
-    <row r="456" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A456" s="4">
         <v>454</v>
       </c>
@@ -38239,7 +38230,7 @@
         <v>24.3922916910028</v>
       </c>
     </row>
-    <row r="457" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A457" s="4">
         <v>455</v>
       </c>
@@ -38321,7 +38312,7 @@
         <v>25.052390563449102</v>
       </c>
     </row>
-    <row r="458" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A458" s="4">
         <v>456</v>
       </c>
@@ -38403,7 +38394,7 @@
         <v>26.2077623299962</v>
       </c>
     </row>
-    <row r="459" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A459" s="4">
         <v>457</v>
       </c>
@@ -38485,7 +38476,7 @@
         <v>27.435884325085102</v>
       </c>
     </row>
-    <row r="460" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A460" s="4">
         <v>458</v>
       </c>
@@ -38567,7 +38558,7 @@
         <v>28.5370556655485</v>
       </c>
     </row>
-    <row r="461" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A461" s="4">
         <v>459</v>
       </c>
@@ -38649,7 +38640,7 @@
         <v>30.907045423627299</v>
       </c>
     </row>
-    <row r="462" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A462" s="4">
         <v>460</v>
       </c>
@@ -38731,7 +38722,7 @@
         <v>33.586863040948401</v>
       </c>
     </row>
-    <row r="463" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A463" s="4">
         <v>461</v>
       </c>
@@ -38813,7 +38804,7 @@
         <v>35.035803606518698</v>
       </c>
     </row>
-    <row r="464" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A464" s="4">
         <v>462</v>
       </c>
@@ -38895,7 +38886,7 @@
         <v>36.293336032319701</v>
       </c>
     </row>
-    <row r="465" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A465" s="4">
         <v>463</v>
       </c>
@@ -38977,7 +38968,7 @@
         <v>36.319274648816197</v>
       </c>
     </row>
-    <row r="466" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A466" s="4">
         <v>464</v>
       </c>
@@ -39059,7 +39050,7 @@
         <v>36.2749183166666</v>
       </c>
     </row>
-    <row r="467" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A467" s="4">
         <v>465</v>
       </c>
@@ -39141,7 +39132,7 @@
         <v>36.221345245740899</v>
       </c>
     </row>
-    <row r="468" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A468" s="4">
         <v>466</v>
       </c>
@@ -39223,7 +39214,7 @@
         <v>35.285229299660898</v>
       </c>
     </row>
-    <row r="469" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A469" s="4">
         <v>467</v>
       </c>
@@ -39305,7 +39296,7 @@
         <v>34.491844671828403</v>
       </c>
     </row>
-    <row r="470" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A470" s="4">
         <v>468</v>
       </c>
@@ -39387,7 +39378,7 @@
         <v>34.539741210403903</v>
       </c>
     </row>
-    <row r="471" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A471" s="4">
         <v>469</v>
       </c>
@@ -39469,7 +39460,7 @@
         <v>35.215494782381597</v>
       </c>
     </row>
-    <row r="472" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A472" s="4">
         <v>470</v>
       </c>
@@ -39551,7 +39542,7 @@
         <v>35.912930159901897</v>
       </c>
     </row>
-    <row r="473" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A473" s="4">
         <v>471</v>
       </c>
@@ -39633,7 +39624,7 @@
         <v>36.983497102724797</v>
       </c>
     </row>
-    <row r="474" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A474" s="4">
         <v>472</v>
       </c>
@@ -39715,7 +39706,7 @@
         <v>38.187671721008201</v>
       </c>
     </row>
-    <row r="475" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A475" s="4">
         <v>473</v>
       </c>
@@ -39797,7 +39788,7 @@
         <v>39.099087402643597</v>
       </c>
     </row>
-    <row r="476" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A476" s="4">
         <v>474</v>
       </c>
@@ -39879,7 +39870,7 @@
         <v>39.172245084957801</v>
       </c>
     </row>
-    <row r="477" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A477" s="4">
         <v>475</v>
       </c>
@@ -39961,7 +39952,7 @@
         <v>39.492990098616197</v>
       </c>
     </row>
-    <row r="478" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A478" s="4">
         <v>476</v>
       </c>
@@ -40043,7 +40034,7 @@
         <v>39.496202088094599</v>
       </c>
     </row>
-    <row r="479" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A479" s="4">
         <v>477</v>
       </c>
@@ -40125,7 +40116,7 @@
         <v>39.624171734112402</v>
       </c>
     </row>
-    <row r="480" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A480" s="4">
         <v>478</v>
       </c>
@@ -40207,7 +40198,7 @@
         <v>38.991812702546298</v>
       </c>
     </row>
-    <row r="481" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A481" s="4">
         <v>479</v>
       </c>
@@ -40289,7 +40280,7 @@
         <v>37.411146186790901</v>
       </c>
     </row>
-    <row r="482" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A482" s="4">
         <v>480</v>
       </c>
@@ -40371,7 +40362,7 @@
         <v>35.048205196674999</v>
       </c>
     </row>
-    <row r="483" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A483" s="4">
         <v>481</v>
       </c>
@@ -40453,7 +40444,7 @@
         <v>33.114286217894701</v>
       </c>
     </row>
-    <row r="484" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A484" s="4">
         <v>482</v>
       </c>
@@ -40535,7 +40526,7 @@
         <v>31.660245288681502</v>
       </c>
     </row>
-    <row r="485" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A485" s="4">
         <v>483</v>
       </c>
@@ -40617,7 +40608,7 @@
         <v>30.7003919657691</v>
       </c>
     </row>
-    <row r="486" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A486" s="4">
         <v>484</v>
       </c>
@@ -40699,7 +40690,7 @@
         <v>30.074803034748701</v>
       </c>
     </row>
-    <row r="487" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A487" s="4">
         <v>485</v>
       </c>
@@ -40781,7 +40772,7 @@
         <v>30.169507806168099</v>
       </c>
     </row>
-    <row r="488" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A488" s="4">
         <v>486</v>
       </c>
@@ -40863,7 +40854,7 @@
         <v>29.910825236138699</v>
       </c>
     </row>
-    <row r="489" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A489" s="4">
         <v>487</v>
       </c>
@@ -40945,7 +40936,7 @@
         <v>30.2008063990999</v>
       </c>
     </row>
-    <row r="490" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A490" s="4">
         <v>488</v>
       </c>
@@ -41027,7 +41018,7 @@
         <v>30.505063722257201</v>
       </c>
     </row>
-    <row r="491" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A491" s="4">
         <v>489</v>
       </c>
@@ -41109,7 +41100,7 @@
         <v>30.638516125959701</v>
       </c>
     </row>
-    <row r="492" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A492" s="4">
         <v>490</v>
       </c>
@@ -41191,7 +41182,7 @@
         <v>30.983166642136901</v>
       </c>
     </row>
-    <row r="493" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A493" s="4">
         <v>491</v>
       </c>
@@ -41273,7 +41264,7 @@
         <v>31.0967744154316</v>
       </c>
     </row>
-    <row r="494" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A494" s="4">
         <v>492</v>
       </c>
@@ -41355,7 +41346,7 @@
         <v>31.463819131952899</v>
       </c>
     </row>
-    <row r="495" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A495" s="4">
         <v>493</v>
       </c>
@@ -41437,7 +41428,7 @@
         <v>30.938772501267199</v>
       </c>
     </row>
-    <row r="496" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A496" s="4">
         <v>494</v>
       </c>
@@ -41519,7 +41510,7 @@
         <v>30.535927713522199</v>
       </c>
     </row>
-    <row r="497" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A497" s="4">
         <v>495</v>
       </c>
@@ -41601,7 +41592,7 @@
         <v>30.282776040365199</v>
       </c>
     </row>
-    <row r="498" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A498" s="4">
         <v>496</v>
       </c>
@@ -41683,7 +41674,7 @@
         <v>30.497836595735201</v>
       </c>
     </row>
-    <row r="499" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A499" s="4">
         <v>497</v>
       </c>
@@ -41765,7 +41756,7 @@
         <v>30.912779117799101</v>
       </c>
     </row>
-    <row r="500" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A500" s="4">
         <v>498</v>
       </c>
@@ -41847,7 +41838,7 @@
         <v>31.2099596113381</v>
       </c>
     </row>
-    <row r="501" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A501" s="4">
         <v>499</v>
       </c>
@@ -41929,7 +41920,7 @@
         <v>31.113824222237</v>
       </c>
     </row>
-    <row r="502" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A502" s="4">
         <v>500</v>
       </c>
@@ -42011,7 +42002,7 @@
         <v>30.960371035230398</v>
       </c>
     </row>
-    <row r="503" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A503" s="4">
         <v>501</v>
       </c>
@@ -42059,7 +42050,7 @@
         <f>100*testdata[[#This Row],[-DM14]]/testdata[[#This Row],[TR14]]</f>
         <v>31.150968674636061</v>
       </c>
-      <c r="N503" s="6">
+      <c r="N503" s="11">
         <f>100*ABS(testdata[[#This Row],[+DI14]]-testdata[[#This Row],[-DI14]])/(testdata[[#This Row],[+DI14]]+testdata[[#This Row],[-DI14]])</f>
         <v>27.387308306629919</v>
       </c>

</xml_diff>

<commit_message>
feat: Buffer-style ADX incremental (#1271)
</commit_message>
<xml_diff>
--- a/tests/indicators/a-d/Adx/Adx.Calc.xlsx
+++ b/tests/indicators/a-d/Adx/Adx.Calc.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1D8B8F-9F53-4B0A-A856-4006463BEA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3415FB2C-712A-4184-A87B-956C4B37A34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36480" yWindow="0" windowWidth="28800" windowHeight="21690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ADX" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -607,7 +598,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1549,22 +1540,22 @@
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="12" max="16" width="9.140625" style="7"/>
-    <col min="17" max="17" width="3.7109375" customWidth="1"/>
-    <col min="18" max="18" width="8.140625" style="5" customWidth="1"/>
-    <col min="19" max="21" width="9.140625" style="7"/>
-    <col min="23" max="23" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="9.140625" style="7"/>
+    <col min="9" max="9" width="9.1796875" customWidth="1"/>
+    <col min="12" max="16" width="9.1796875" style="7"/>
+    <col min="17" max="17" width="3.7265625" customWidth="1"/>
+    <col min="18" max="18" width="8.1796875" style="5" customWidth="1"/>
+    <col min="19" max="21" width="9.1796875" style="7"/>
+    <col min="23" max="23" width="8.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="9.1796875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -1635,7 +1626,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -1674,7 +1665,7 @@
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1722,7 +1713,7 @@
       <c r="X3" s="6"/>
       <c r="Y3" s="6"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -1770,7 +1761,7 @@
       <c r="X4" s="6"/>
       <c r="Y4" s="6"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1818,7 +1809,7 @@
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1866,7 +1857,7 @@
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1914,7 +1905,7 @@
       <c r="X7" s="6"/>
       <c r="Y7" s="6"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1962,7 +1953,7 @@
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -2010,7 +2001,7 @@
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -2058,7 +2049,7 @@
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -2106,7 +2097,7 @@
       <c r="X11" s="6"/>
       <c r="Y11" s="6"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -2154,7 +2145,7 @@
       <c r="X12" s="6"/>
       <c r="Y12" s="6"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -2202,7 +2193,7 @@
       <c r="X13" s="6"/>
       <c r="Y13" s="6"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -2250,7 +2241,7 @@
       <c r="X14" s="6"/>
       <c r="Y14" s="6"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -2298,7 +2289,7 @@
       <c r="X15" s="6"/>
       <c r="Y15" s="6"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -2368,7 +2359,7 @@
       <c r="X16" s="6"/>
       <c r="Y16" s="6"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -2438,7 +2429,7 @@
       <c r="X17" s="6"/>
       <c r="Y17" s="6"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -2508,7 +2499,7 @@
       <c r="X18" s="6"/>
       <c r="Y18" s="6"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -2578,7 +2569,7 @@
       <c r="X19" s="6"/>
       <c r="Y19" s="6"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -2648,7 +2639,7 @@
       <c r="X20" s="6"/>
       <c r="Y20" s="6"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -2696,7 +2687,7 @@
         <f>100*testdata[[#This Row],[-DM14]]/testdata[[#This Row],[TR14]]</f>
         <v>25.012425579421205</v>
       </c>
-      <c r="N21" s="6">
+      <c r="N21" s="11">
         <f>100*ABS(testdata[[#This Row],[+DI14]]-testdata[[#This Row],[-DI14]])/(testdata[[#This Row],[+DI14]]+testdata[[#This Row],[-DI14]])</f>
         <v>8.6351139279442961</v>
       </c>
@@ -2718,7 +2709,7 @@
       <c r="X21" s="11"/>
       <c r="Y21" s="11"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -2788,7 +2779,7 @@
       <c r="X22" s="6"/>
       <c r="Y22" s="6"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -2858,7 +2849,7 @@
       <c r="X23" s="6"/>
       <c r="Y23" s="6"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -2928,7 +2919,7 @@
       <c r="X24" s="6"/>
       <c r="Y24" s="6"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -2998,7 +2989,7 @@
       <c r="X25" s="6"/>
       <c r="Y25" s="6"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -3068,7 +3059,7 @@
       <c r="X26" s="6"/>
       <c r="Y26" s="6"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -3138,7 +3129,7 @@
       <c r="X27" s="6"/>
       <c r="Y27" s="6"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -3208,7 +3199,7 @@
       <c r="X28" s="6"/>
       <c r="Y28" s="6"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -3285,7 +3276,7 @@
       </c>
       <c r="Y29" s="13"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -3362,7 +3353,7 @@
       </c>
       <c r="Y30" s="6"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -3410,7 +3401,7 @@
         <f>100*testdata[[#This Row],[-DM14]]/testdata[[#This Row],[TR14]]</f>
         <v>14.165829841353299</v>
       </c>
-      <c r="N31" s="6">
+      <c r="N31" s="11">
         <f>100*ABS(testdata[[#This Row],[+DI14]]-testdata[[#This Row],[-DI14]])/(testdata[[#This Row],[+DI14]]+testdata[[#This Row],[-DI14]])</f>
         <v>45.659962116806589</v>
       </c>
@@ -3439,7 +3430,7 @@
       </c>
       <c r="Y31" s="11"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -3516,7 +3507,7 @@
       </c>
       <c r="Y32" s="6"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -3593,7 +3584,7 @@
       </c>
       <c r="Y33" s="6"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -3670,7 +3661,7 @@
       </c>
       <c r="Y34" s="6"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>33</v>
       </c>
@@ -3747,7 +3738,7 @@
       </c>
       <c r="Y35" s="6"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -3824,7 +3815,7 @@
       </c>
       <c r="Y36" s="6"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -3901,7 +3892,7 @@
       </c>
       <c r="Y37" s="6"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -3978,7 +3969,7 @@
       </c>
       <c r="Y38" s="6"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -4055,7 +4046,7 @@
       </c>
       <c r="Y39" s="6"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -4132,7 +4123,7 @@
       </c>
       <c r="Y40" s="6"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -4209,7 +4200,7 @@
       </c>
       <c r="Y41" s="6"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -4291,7 +4282,7 @@
         <v>29.1061924422517</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -4373,7 +4364,7 @@
         <v>30.612091066317898</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -4455,7 +4446,7 @@
         <v>31.742940902605799</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -4537,7 +4528,7 @@
         <v>32.910704164193803</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -4619,7 +4610,7 @@
         <v>33.800668233057998</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -4701,7 +4692,7 @@
         <v>34.282530871755498</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -4783,7 +4774,7 @@
         <v>35.203773847973203</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -4865,7 +4856,7 @@
         <v>36.059213754461098</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -4947,7 +4938,7 @@
         <v>36.365003212984099</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -5029,7 +5020,7 @@
         <v>37.142611710382397</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -5111,7 +5102,7 @@
         <v>37.952532158976197</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -5193,7 +5184,7 @@
         <v>38.4561721826583</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -5275,7 +5266,7 @@
         <v>39.044472480502797</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -5357,7 +5348,7 @@
         <v>38.805876785297102</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -5439,7 +5430,7 @@
         <v>38.471016752236899</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A57" s="4">
         <v>55</v>
       </c>
@@ -5521,7 +5512,7 @@
         <v>37.4997691385419</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A58" s="4">
         <v>56</v>
       </c>
@@ -5603,7 +5594,7 @@
         <v>36.665467018523003</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A59" s="4">
         <v>57</v>
       </c>
@@ -5685,7 +5676,7 @@
         <v>36.079144579880399</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A60" s="4">
         <v>58</v>
       </c>
@@ -5767,7 +5758,7 @@
         <v>34.551715527415404</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A61" s="4">
         <v>59</v>
       </c>
@@ -5849,7 +5840,7 @@
         <v>33.344820747917403</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A62" s="4">
         <v>60</v>
       </c>
@@ -5931,7 +5922,7 @@
         <v>32.366541473105897</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A63" s="4">
         <v>61</v>
       </c>
@@ -6013,7 +6004,7 @@
         <v>30.914364787662802</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A64" s="4">
         <v>62</v>
       </c>
@@ -6095,7 +6086,7 @@
         <v>30.357705712508601</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A65" s="4">
         <v>63</v>
       </c>
@@ -6177,7 +6168,7 @@
         <v>29.840807999865401</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A66" s="4">
         <v>64</v>
       </c>
@@ -6259,7 +6250,7 @@
         <v>29.172918215714301</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A67" s="4">
         <v>65</v>
       </c>
@@ -6341,7 +6332,7 @@
         <v>28.1491072195229</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A68" s="4">
         <v>66</v>
       </c>
@@ -6423,7 +6414,7 @@
         <v>26.504759350980599</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A69" s="4">
         <v>67</v>
       </c>
@@ -6505,7 +6496,7 @@
         <v>25.231445672096498</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A70" s="4">
         <v>68</v>
       </c>
@@ -6587,7 +6578,7 @@
         <v>23.7548435583547</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A71" s="4">
         <v>69</v>
       </c>
@@ -6669,7 +6660,7 @@
         <v>22.5885590108646</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A72" s="4">
         <v>70</v>
       </c>
@@ -6751,7 +6742,7 @@
         <v>22.295802015566402</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A73" s="4">
         <v>71</v>
       </c>
@@ -6833,7 +6824,7 @@
         <v>21.349036701747899</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A74" s="4">
         <v>72</v>
       </c>
@@ -6915,7 +6906,7 @@
         <v>20.4698974817737</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A75" s="4">
         <v>73</v>
       </c>
@@ -6997,7 +6988,7 @@
         <v>19.577440110008901</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A76" s="4">
         <v>74</v>
       </c>
@@ -7079,7 +7070,7 @@
         <v>18.364523548171501</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A77" s="4">
         <v>75</v>
       </c>
@@ -7161,7 +7152,7 @@
         <v>17.4385494803442</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A78" s="4">
         <v>76</v>
       </c>
@@ -7243,7 +7234,7 @@
         <v>17.329884510539799</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A79" s="4">
         <v>77</v>
       </c>
@@ -7325,7 +7316,7 @@
         <v>17.4648063151473</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A80" s="4">
         <v>78</v>
       </c>
@@ -7407,7 +7398,7 @@
         <v>17.682948149028899</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A81" s="4">
         <v>79</v>
       </c>
@@ -7489,7 +7480,7 @@
         <v>17.7100214417076</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A82" s="4">
         <v>80</v>
       </c>
@@ -7571,7 +7562,7 @@
         <v>17.799489278081499</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A83" s="4">
         <v>81</v>
       </c>
@@ -7653,7 +7644,7 @@
         <v>17.915875466956699</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A84" s="4">
         <v>82</v>
       </c>
@@ -7735,7 +7726,7 @@
         <v>18.023948356626502</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A85" s="4">
         <v>83</v>
       </c>
@@ -7817,7 +7808,7 @@
         <v>18.1939708200286</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A86" s="4">
         <v>84</v>
       </c>
@@ -7899,7 +7890,7 @@
         <v>18.333775819821199</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A87" s="4">
         <v>85</v>
       </c>
@@ -7981,7 +7972,7 @@
         <v>18.729992570185601</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A88" s="4">
         <v>86</v>
       </c>
@@ -8063,7 +8054,7 @@
         <v>18.943293212509801</v>
       </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A89" s="4">
         <v>87</v>
       </c>
@@ -8145,7 +8136,7 @@
         <v>18.845526482244999</v>
       </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A90" s="4">
         <v>88</v>
       </c>
@@ -8227,7 +8218,7 @@
         <v>18.754743089856301</v>
       </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A91" s="4">
         <v>89</v>
       </c>
@@ -8309,7 +8300,7 @@
         <v>18.760152884100101</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A92" s="4">
         <v>90</v>
       </c>
@@ -8391,7 +8382,7 @@
         <v>19.1669628391214</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A93" s="4">
         <v>91</v>
       </c>
@@ -8473,7 +8464,7 @@
         <v>20.081985790329501</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A94" s="4">
         <v>92</v>
       </c>
@@ -8555,7 +8546,7 @@
         <v>20.836070292675601</v>
       </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A95" s="4">
         <v>93</v>
       </c>
@@ -8637,7 +8628,7 @@
         <v>21.073811681227099</v>
       </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A96" s="4">
         <v>94</v>
       </c>
@@ -8719,7 +8710,7 @@
         <v>21.455839944231698</v>
       </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A97" s="4">
         <v>95</v>
       </c>
@@ -8801,7 +8792,7 @@
         <v>21.2716280780853</v>
       </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A98" s="4">
         <v>96</v>
       </c>
@@ -8883,7 +8874,7 @@
         <v>20.5940638953319</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A99" s="4">
         <v>97</v>
       </c>
@@ -8965,7 +8956,7 @@
         <v>20.167656670205499</v>
       </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A100" s="4">
         <v>98</v>
       </c>
@@ -9047,7 +9038,7 @@
         <v>20.199714171617</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A101" s="4">
         <v>99</v>
       </c>
@@ -9129,7 +9120,7 @@
         <v>20.696337137899501</v>
       </c>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A102" s="4">
         <v>100</v>
       </c>
@@ -9211,7 +9202,7 @@
         <v>21.245861567937698</v>
       </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A103" s="4">
         <v>101</v>
       </c>
@@ -9293,7 +9284,7 @@
         <v>21.6262416569778</v>
       </c>
     </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A104" s="4">
         <v>102</v>
       </c>
@@ -9375,7 +9366,7 @@
         <v>21.085307012226501</v>
       </c>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A105" s="4">
         <v>103</v>
       </c>
@@ -9457,7 +9448,7 @@
         <v>21.049995180387899</v>
       </c>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A106" s="4">
         <v>104</v>
       </c>
@@ -9539,7 +9530,7 @@
         <v>21.672467470452801</v>
       </c>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A107" s="4">
         <v>105</v>
       </c>
@@ -9621,7 +9612,7 @@
         <v>22.330384769091701</v>
       </c>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A108" s="4">
         <v>106</v>
       </c>
@@ -9703,7 +9694,7 @@
         <v>22.191305661936902</v>
       </c>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A109" s="4">
         <v>107</v>
       </c>
@@ -9785,7 +9776,7 @@
         <v>22.017220872573901</v>
       </c>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A110" s="4">
         <v>108</v>
       </c>
@@ -9867,7 +9858,7 @@
         <v>21.448871413869199</v>
       </c>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A111" s="4">
         <v>109</v>
       </c>
@@ -9949,7 +9940,7 @@
         <v>20.1916776939816</v>
       </c>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A112" s="4">
         <v>110</v>
       </c>
@@ -10031,7 +10022,7 @@
         <v>19.208650730890302</v>
       </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A113" s="4">
         <v>111</v>
       </c>
@@ -10113,7 +10104,7 @@
         <v>18.876123557151701</v>
       </c>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A114" s="4">
         <v>112</v>
       </c>
@@ -10195,7 +10186,7 @@
         <v>18.8323775209107</v>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A115" s="4">
         <v>113</v>
       </c>
@@ -10277,7 +10268,7 @@
         <v>18.384938741852299</v>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A116" s="4">
         <v>114</v>
       </c>
@@ -10359,7 +10350,7 @@
         <v>17.880924714904499</v>
       </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A117" s="4">
         <v>115</v>
       </c>
@@ -10441,7 +10432,7 @@
         <v>17.8257912322909</v>
       </c>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A118" s="4">
         <v>116</v>
       </c>
@@ -10523,7 +10514,7 @@
         <v>18.021104841539</v>
       </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A119" s="4">
         <v>117</v>
       </c>
@@ -10605,7 +10596,7 @@
         <v>18.204445089235399</v>
       </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A120" s="4">
         <v>118</v>
       </c>
@@ -10687,7 +10678,7 @@
         <v>18.374689604953399</v>
       </c>
     </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A121" s="4">
         <v>119</v>
       </c>
@@ -10769,7 +10760,7 @@
         <v>18.1374786511679</v>
       </c>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A122" s="4">
         <v>120</v>
       </c>
@@ -10851,7 +10842,7 @@
         <v>18.105568195448399</v>
       </c>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A123" s="4">
         <v>121</v>
       </c>
@@ -10933,7 +10924,7 @@
         <v>17.760763803450999</v>
       </c>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A124" s="4">
         <v>122</v>
       </c>
@@ -11015,7 +11006,7 @@
         <v>16.7507030014878</v>
       </c>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A125" s="4">
         <v>123</v>
       </c>
@@ -11097,7 +11088,7 @@
         <v>16.542459502739199</v>
       </c>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A126" s="4">
         <v>124</v>
       </c>
@@ -11179,7 +11170,7 @@
         <v>16.767764871704099</v>
       </c>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A127" s="4">
         <v>125</v>
       </c>
@@ -11261,7 +11252,7 @@
         <v>16.556801427059099</v>
       </c>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A128" s="4">
         <v>126</v>
       </c>
@@ -11343,7 +11334,7 @@
         <v>16.113631331442001</v>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A129" s="4">
         <v>127</v>
       </c>
@@ -11425,7 +11416,7 @@
         <v>16.120742708005</v>
       </c>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A130" s="4">
         <v>128</v>
       </c>
@@ -11507,7 +11498,7 @@
         <v>16.6599037100797</v>
       </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A131" s="4">
         <v>129</v>
       </c>
@@ -11589,7 +11580,7 @@
         <v>16.705822336562999</v>
       </c>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A132" s="4">
         <v>130</v>
       </c>
@@ -11671,7 +11662,7 @@
         <v>16.7628409089901</v>
       </c>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A133" s="4">
         <v>131</v>
       </c>
@@ -11753,7 +11744,7 @@
         <v>16.150396947228401</v>
       </c>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A134" s="4">
         <v>132</v>
       </c>
@@ -11835,7 +11826,7 @@
         <v>15.3720936341465</v>
       </c>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A135" s="4">
         <v>133</v>
       </c>
@@ -11917,7 +11908,7 @@
         <v>15.207804271541301</v>
       </c>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A136" s="4">
         <v>134</v>
       </c>
@@ -11999,7 +11990,7 @@
         <v>14.607823509938299</v>
       </c>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A137" s="4">
         <v>135</v>
       </c>
@@ -12081,7 +12072,7 @@
         <v>13.6711197999911</v>
       </c>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A138" s="4">
         <v>136</v>
       </c>
@@ -12163,7 +12154,7 @@
         <v>13.937102595633201</v>
       </c>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A139" s="4">
         <v>137</v>
       </c>
@@ -12245,7 +12236,7 @@
         <v>14.305698275808799</v>
       </c>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A140" s="4">
         <v>138</v>
       </c>
@@ -12327,7 +12318,7 @@
         <v>14.243953693353401</v>
       </c>
     </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A141" s="4">
         <v>139</v>
       </c>
@@ -12409,7 +12400,7 @@
         <v>14.366568041736301</v>
       </c>
     </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A142" s="4">
         <v>140</v>
       </c>
@@ -12491,7 +12482,7 @@
         <v>15.1203531340515</v>
       </c>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A143" s="4">
         <v>141</v>
       </c>
@@ -12573,7 +12564,7 @@
         <v>15.691984664705901</v>
       </c>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A144" s="4">
         <v>142</v>
       </c>
@@ -12655,7 +12646,7 @@
         <v>15.3449938541245</v>
       </c>
     </row>
-    <row r="145" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A145" s="4">
         <v>143</v>
       </c>
@@ -12737,7 +12728,7 @@
         <v>15.285300670218</v>
       </c>
     </row>
-    <row r="146" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A146" s="4">
         <v>144</v>
       </c>
@@ -12819,7 +12810,7 @@
         <v>14.727913284457699</v>
       </c>
     </row>
-    <row r="147" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A147" s="4">
         <v>145</v>
       </c>
@@ -12901,7 +12892,7 @@
         <v>14.090988831051201</v>
       </c>
     </row>
-    <row r="148" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A148" s="4">
         <v>146</v>
       </c>
@@ -12983,7 +12974,7 @@
         <v>13.561939402961</v>
       </c>
     </row>
-    <row r="149" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A149" s="4">
         <v>147</v>
       </c>
@@ -13065,7 +13056,7 @@
         <v>13.070679219734499</v>
       </c>
     </row>
-    <row r="150" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A150" s="4">
         <v>148</v>
       </c>
@@ -13147,7 +13138,7 @@
         <v>12.5772595112294</v>
       </c>
     </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A151" s="4">
         <v>149</v>
       </c>
@@ -13229,7 +13220,7 @@
         <v>12.5596040027716</v>
       </c>
     </row>
-    <row r="152" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A152" s="4">
         <v>150</v>
       </c>
@@ -13311,7 +13302,7 @@
         <v>13.110921462571101</v>
       </c>
     </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A153" s="4">
         <v>151</v>
       </c>
@@ -13393,7 +13384,7 @@
         <v>13.062343953195899</v>
       </c>
     </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A154" s="4">
         <v>152</v>
       </c>
@@ -13475,7 +13466,7 @@
         <v>13.252946001101799</v>
       </c>
     </row>
-    <row r="155" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A155" s="4">
         <v>153</v>
       </c>
@@ -13557,7 +13548,7 @@
         <v>13.692593498654</v>
       </c>
     </row>
-    <row r="156" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A156" s="4">
         <v>154</v>
       </c>
@@ -13639,7 +13630,7 @@
         <v>13.699636441906801</v>
       </c>
     </row>
-    <row r="157" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A157" s="4">
         <v>155</v>
       </c>
@@ -13721,7 +13712,7 @@
         <v>13.1356829936324</v>
       </c>
     </row>
-    <row r="158" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A158" s="4">
         <v>156</v>
       </c>
@@ -13803,7 +13794,7 @@
         <v>12.8108158536141</v>
       </c>
     </row>
-    <row r="159" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A159" s="4">
         <v>157</v>
       </c>
@@ -13885,7 +13876,7 @@
         <v>12.816410100620899</v>
       </c>
     </row>
-    <row r="160" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A160" s="4">
         <v>158</v>
       </c>
@@ -13967,7 +13958,7 @@
         <v>13.044485021236101</v>
       </c>
     </row>
-    <row r="161" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A161" s="4">
         <v>159</v>
       </c>
@@ -14049,7 +14040,7 @@
         <v>13.1763539087168</v>
       </c>
     </row>
-    <row r="162" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A162" s="4">
         <v>160</v>
       </c>
@@ -14131,7 +14122,7 @@
         <v>12.479310573888</v>
       </c>
     </row>
-    <row r="163" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A163" s="4">
         <v>161</v>
       </c>
@@ -14213,7 +14204,7 @@
         <v>12.0434436761443</v>
       </c>
     </row>
-    <row r="164" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A164" s="4">
         <v>162</v>
       </c>
@@ -14295,7 +14286,7 @@
         <v>11.7950640075442</v>
       </c>
     </row>
-    <row r="165" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A165" s="4">
         <v>163</v>
       </c>
@@ -14377,7 +14368,7 @@
         <v>11.8679599910823</v>
       </c>
     </row>
-    <row r="166" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A166" s="4">
         <v>164</v>
       </c>
@@ -14459,7 +14450,7 @@
         <v>11.5901761420778</v>
       </c>
     </row>
-    <row r="167" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A167" s="4">
         <v>165</v>
       </c>
@@ -14541,7 +14532,7 @@
         <v>11.895316982337601</v>
       </c>
     </row>
-    <row r="168" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A168" s="4">
         <v>166</v>
       </c>
@@ -14623,7 +14614,7 @@
         <v>11.7665845155101</v>
       </c>
     </row>
-    <row r="169" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A169" s="4">
         <v>167</v>
       </c>
@@ -14705,7 +14696,7 @@
         <v>11.453332262058799</v>
       </c>
     </row>
-    <row r="170" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A170" s="4">
         <v>168</v>
       </c>
@@ -14787,7 +14778,7 @@
         <v>11.386578842492</v>
       </c>
     </row>
-    <row r="171" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A171" s="4">
         <v>169</v>
       </c>
@@ -14869,7 +14860,7 @@
         <v>11.3865920698675</v>
       </c>
     </row>
-    <row r="172" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A172" s="4">
         <v>170</v>
       </c>
@@ -14951,7 +14942,7 @@
         <v>11.530429165428901</v>
       </c>
     </row>
-    <row r="173" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A173" s="4">
         <v>171</v>
       </c>
@@ -15033,7 +15024,7 @@
         <v>11.8785112450217</v>
       </c>
     </row>
-    <row r="174" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A174" s="4">
         <v>172</v>
       </c>
@@ -15115,7 +15106,7 @@
         <v>12.316903208731601</v>
       </c>
     </row>
-    <row r="175" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A175" s="4">
         <v>173</v>
       </c>
@@ -15197,7 +15188,7 @@
         <v>11.879291358187199</v>
       </c>
     </row>
-    <row r="176" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A176" s="4">
         <v>174</v>
       </c>
@@ -15279,7 +15270,7 @@
         <v>11.6775344168566</v>
       </c>
     </row>
-    <row r="177" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A177" s="4">
         <v>175</v>
       </c>
@@ -15361,7 +15352,7 @@
         <v>11.642109123715301</v>
       </c>
     </row>
-    <row r="178" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A178" s="4">
         <v>176</v>
       </c>
@@ -15443,7 +15434,7 @@
         <v>11.498276887877999</v>
       </c>
     </row>
-    <row r="179" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A179" s="4">
         <v>177</v>
       </c>
@@ -15525,7 +15516,7 @@
         <v>11.5180480427939</v>
       </c>
     </row>
-    <row r="180" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A180" s="4">
         <v>178</v>
       </c>
@@ -15607,7 +15598,7 @@
         <v>12.1146615703083</v>
       </c>
     </row>
-    <row r="181" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A181" s="4">
         <v>179</v>
       </c>
@@ -15689,7 +15680,7 @@
         <v>12.2565823130744</v>
       </c>
     </row>
-    <row r="182" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A182" s="4">
         <v>180</v>
       </c>
@@ -15771,7 +15762,7 @@
         <v>12.2678793832705</v>
       </c>
     </row>
-    <row r="183" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A183" s="4">
         <v>181</v>
       </c>
@@ -15853,7 +15844,7 @@
         <v>12.4294502367413</v>
       </c>
     </row>
-    <row r="184" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A184" s="4">
         <v>182</v>
       </c>
@@ -15935,7 +15926,7 @@
         <v>12.361304498200401</v>
       </c>
     </row>
-    <row r="185" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A185" s="4">
         <v>183</v>
       </c>
@@ -16017,7 +16008,7 @@
         <v>11.866143483161499</v>
       </c>
     </row>
-    <row r="186" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A186" s="4">
         <v>184</v>
       </c>
@@ -16099,7 +16090,7 @@
         <v>11.467767805282801</v>
       </c>
     </row>
-    <row r="187" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A187" s="4">
         <v>185</v>
       </c>
@@ -16181,7 +16172,7 @@
         <v>11.445273740109201</v>
       </c>
     </row>
-    <row r="188" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A188" s="4">
         <v>186</v>
       </c>
@@ -16263,7 +16254,7 @@
         <v>11.3991893073767</v>
       </c>
     </row>
-    <row r="189" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A189" s="4">
         <v>187</v>
       </c>
@@ -16345,7 +16336,7 @@
         <v>11.8936194473648</v>
       </c>
     </row>
-    <row r="190" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A190" s="4">
         <v>188</v>
       </c>
@@ -16427,7 +16418,7 @@
         <v>12.7062609107585</v>
       </c>
     </row>
-    <row r="191" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A191" s="4">
         <v>189</v>
       </c>
@@ -16509,7 +16500,7 @@
         <v>13.6572585725811</v>
       </c>
     </row>
-    <row r="192" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A192" s="4">
         <v>190</v>
       </c>
@@ -16591,7 +16582,7 @@
         <v>14.747016123276699</v>
       </c>
     </row>
-    <row r="193" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A193" s="4">
         <v>191</v>
       </c>
@@ -16673,7 +16664,7 @@
         <v>16.282048374839999</v>
       </c>
     </row>
-    <row r="194" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A194" s="4">
         <v>192</v>
       </c>
@@ -16755,7 +16746,7 @@
         <v>17.712003983233199</v>
       </c>
     </row>
-    <row r="195" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A195" s="4">
         <v>193</v>
       </c>
@@ -16837,7 +16828,7 @@
         <v>18.5918000980394</v>
       </c>
     </row>
-    <row r="196" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A196" s="4">
         <v>194</v>
       </c>
@@ -16919,7 +16910,7 @@
         <v>19.498445742313798</v>
       </c>
     </row>
-    <row r="197" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A197" s="4">
         <v>195</v>
       </c>
@@ -17001,7 +16992,7 @@
         <v>20.2589605402109</v>
       </c>
     </row>
-    <row r="198" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A198" s="4">
         <v>196</v>
       </c>
@@ -17083,7 +17074,7 @@
         <v>20.544887992854999</v>
       </c>
     </row>
-    <row r="199" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A199" s="4">
         <v>197</v>
       </c>
@@ -17165,7 +17156,7 @@
         <v>20.932015121038699</v>
       </c>
     </row>
-    <row r="200" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A200" s="4">
         <v>198</v>
       </c>
@@ -17247,7 +17238,7 @@
         <v>21.681003499998699</v>
       </c>
     </row>
-    <row r="201" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A201" s="4">
         <v>199</v>
       </c>
@@ -17329,7 +17320,7 @@
         <v>22.379617101271698</v>
       </c>
     </row>
-    <row r="202" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A202" s="4">
         <v>200</v>
       </c>
@@ -17411,7 +17402,7 @@
         <v>23.488704368278199</v>
       </c>
     </row>
-    <row r="203" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A203" s="4">
         <v>201</v>
       </c>
@@ -17493,7 +17484,7 @@
         <v>23.8833827363759</v>
       </c>
     </row>
-    <row r="204" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A204" s="4">
         <v>202</v>
       </c>
@@ -17575,7 +17566,7 @@
         <v>24.870522999988498</v>
       </c>
     </row>
-    <row r="205" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A205" s="4">
         <v>203</v>
       </c>
@@ -17657,7 +17648,7 @@
         <v>26.040624648346299</v>
       </c>
     </row>
-    <row r="206" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A206" s="4">
         <v>204</v>
       </c>
@@ -17739,7 +17730,7 @@
         <v>27.419787398359698</v>
       </c>
     </row>
-    <row r="207" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A207" s="4">
         <v>205</v>
       </c>
@@ -17821,7 +17812,7 @@
         <v>27.407198372818101</v>
       </c>
     </row>
-    <row r="208" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A208" s="4">
         <v>206</v>
       </c>
@@ -17903,7 +17894,7 @@
         <v>27.260156916497198</v>
       </c>
     </row>
-    <row r="209" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A209" s="4">
         <v>207</v>
       </c>
@@ -17985,7 +17976,7 @@
         <v>27.811560559992301</v>
       </c>
     </row>
-    <row r="210" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A210" s="4">
         <v>208</v>
       </c>
@@ -18067,7 +18058,7 @@
         <v>28.323578228952101</v>
       </c>
     </row>
-    <row r="211" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A211" s="4">
         <v>209</v>
       </c>
@@ -18149,7 +18140,7 @@
         <v>28.810641176833901</v>
       </c>
     </row>
-    <row r="212" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A212" s="4">
         <v>210</v>
       </c>
@@ -18231,7 +18222,7 @@
         <v>29.654156738617399</v>
       </c>
     </row>
-    <row r="213" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A213" s="4">
         <v>211</v>
       </c>
@@ -18313,7 +18304,7 @@
         <v>30.012186955780201</v>
       </c>
     </row>
-    <row r="214" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A214" s="4">
         <v>212</v>
       </c>
@@ -18395,7 +18386,7 @@
         <v>30.6023842791951</v>
       </c>
     </row>
-    <row r="215" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A215" s="4">
         <v>213</v>
       </c>
@@ -18477,7 +18468,7 @@
         <v>31.4350163904464</v>
       </c>
     </row>
-    <row r="216" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A216" s="4">
         <v>214</v>
       </c>
@@ -18559,7 +18550,7 @@
         <v>31.3571049186111</v>
       </c>
     </row>
-    <row r="217" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A217" s="4">
         <v>215</v>
       </c>
@@ -18641,7 +18632,7 @@
         <v>31.7406383790298</v>
       </c>
     </row>
-    <row r="218" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A218" s="4">
         <v>216</v>
       </c>
@@ -18723,7 +18714,7 @@
         <v>31.238266851310399</v>
       </c>
     </row>
-    <row r="219" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A219" s="4">
         <v>217</v>
       </c>
@@ -18805,7 +18796,7 @@
         <v>30.771779004142399</v>
       </c>
     </row>
-    <row r="220" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A220" s="4">
         <v>218</v>
       </c>
@@ -18887,7 +18878,7 @@
         <v>29.168230146264602</v>
       </c>
     </row>
-    <row r="221" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A221" s="4">
         <v>219</v>
       </c>
@@ -18969,7 +18960,7 @@
         <v>27.3320785577477</v>
       </c>
     </row>
-    <row r="222" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A222" s="4">
         <v>220</v>
       </c>
@@ -19051,7 +19042,7 @@
         <v>26.600198382884098</v>
       </c>
     </row>
-    <row r="223" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A223" s="4">
         <v>221</v>
       </c>
@@ -19133,7 +19124,7 @@
         <v>25.899312218927399</v>
       </c>
     </row>
-    <row r="224" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A224" s="4">
         <v>222</v>
       </c>
@@ -19215,7 +19206,7 @@
         <v>25.248489352396099</v>
       </c>
     </row>
-    <row r="225" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A225" s="4">
         <v>223</v>
       </c>
@@ -19297,7 +19288,7 @@
         <v>24.975190286153602</v>
       </c>
     </row>
-    <row r="226" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A226" s="4">
         <v>224</v>
       </c>
@@ -19379,7 +19370,7 @@
         <v>24.797327877659001</v>
       </c>
     </row>
-    <row r="227" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A227" s="4">
         <v>225</v>
       </c>
@@ -19461,7 +19452,7 @@
         <v>24.886786227867599</v>
       </c>
     </row>
-    <row r="228" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A228" s="4">
         <v>226</v>
       </c>
@@ -19543,7 +19534,7 @@
         <v>25.231215737617799</v>
       </c>
     </row>
-    <row r="229" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A229" s="4">
         <v>227</v>
       </c>
@@ -19625,7 +19616,7 @@
         <v>25.743601967571902</v>
       </c>
     </row>
-    <row r="230" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A230" s="4">
         <v>228</v>
       </c>
@@ -19707,7 +19698,7 @@
         <v>26.763867884306698</v>
       </c>
     </row>
-    <row r="231" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A231" s="4">
         <v>229</v>
       </c>
@@ -19789,7 +19780,7 @@
         <v>26.889232646338399</v>
       </c>
     </row>
-    <row r="232" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A232" s="4">
         <v>230</v>
       </c>
@@ -19871,7 +19862,7 @@
         <v>27.378564049755699</v>
       </c>
     </row>
-    <row r="233" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A233" s="4">
         <v>231</v>
       </c>
@@ -19953,7 +19944,7 @@
         <v>26.722578457910199</v>
       </c>
     </row>
-    <row r="234" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A234" s="4">
         <v>232</v>
       </c>
@@ -20035,7 +20026,7 @@
         <v>26.0433872363791</v>
       </c>
     </row>
-    <row r="235" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A235" s="4">
         <v>233</v>
       </c>
@@ -20117,7 +20108,7 @@
         <v>25.432565694878299</v>
       </c>
     </row>
-    <row r="236" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A236" s="4">
         <v>234</v>
       </c>
@@ -20199,7 +20190,7 @@
         <v>24.736998515986201</v>
       </c>
     </row>
-    <row r="237" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A237" s="4">
         <v>235</v>
       </c>
@@ -20281,7 +20272,7 @@
         <v>24.240650205704</v>
       </c>
     </row>
-    <row r="238" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A238" s="4">
         <v>236</v>
       </c>
@@ -20363,7 +20354,7 @@
         <v>23.9990279894261</v>
       </c>
     </row>
-    <row r="239" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A239" s="4">
         <v>237</v>
       </c>
@@ -20445,7 +20436,7 @@
         <v>24.503548672513901</v>
       </c>
     </row>
-    <row r="240" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A240" s="4">
         <v>238</v>
       </c>
@@ -20527,7 +20518,7 @@
         <v>25.134537340839</v>
       </c>
     </row>
-    <row r="241" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A241" s="4">
         <v>239</v>
       </c>
@@ -20609,7 +20600,7 @@
         <v>25.865718685452102</v>
       </c>
     </row>
-    <row r="242" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A242" s="4">
         <v>240</v>
       </c>
@@ -20691,7 +20682,7 @@
         <v>26.2121296786252</v>
       </c>
     </row>
-    <row r="243" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A243" s="4">
         <v>241</v>
       </c>
@@ -20773,7 +20764,7 @@
         <v>27.306221620894199</v>
       </c>
     </row>
-    <row r="244" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A244" s="4">
         <v>242</v>
       </c>
@@ -20855,7 +20846,7 @@
         <v>28.7289945657628</v>
       </c>
     </row>
-    <row r="245" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A245" s="4">
         <v>243</v>
       </c>
@@ -20937,7 +20928,7 @@
         <v>30.081878929691499</v>
       </c>
     </row>
-    <row r="246" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A246" s="4">
         <v>244</v>
       </c>
@@ -21019,7 +21010,7 @@
         <v>29.953416350638701</v>
       </c>
     </row>
-    <row r="247" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A247" s="4">
         <v>245</v>
       </c>
@@ -21101,7 +21092,7 @@
         <v>30.122000749080701</v>
       </c>
     </row>
-    <row r="248" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A248" s="4">
         <v>246</v>
       </c>
@@ -21183,7 +21174,7 @@
         <v>29.764326961141901</v>
       </c>
     </row>
-    <row r="249" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A249" s="4">
         <v>247</v>
       </c>
@@ -21265,7 +21256,7 @@
         <v>29.316410221164901</v>
       </c>
     </row>
-    <row r="250" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A250" s="4">
         <v>248</v>
       </c>
@@ -21313,7 +21304,7 @@
         <f>100*testdata[[#This Row],[-DM14]]/testdata[[#This Row],[TR14]]</f>
         <v>18.247083794191962</v>
       </c>
-      <c r="N250" s="6">
+      <c r="N250" s="11">
         <f>100*ABS(testdata[[#This Row],[+DI14]]-testdata[[#This Row],[-DI14]])/(testdata[[#This Row],[+DI14]]+testdata[[#This Row],[-DI14]])</f>
         <v>27.825450922906132</v>
       </c>
@@ -21347,7 +21338,7 @@
         <v>29.125166308423101</v>
       </c>
     </row>
-    <row r="251" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A251" s="4">
         <v>249</v>
       </c>
@@ -21429,7 +21420,7 @@
         <v>29.2164317967156</v>
       </c>
     </row>
-    <row r="252" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A252" s="4">
         <v>250</v>
       </c>
@@ -21511,7 +21502,7 @@
         <v>29.079359374489599</v>
       </c>
     </row>
-    <row r="253" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A253" s="4">
         <v>251</v>
       </c>
@@ -21593,7 +21584,7 @@
         <v>29.1949732270187</v>
       </c>
     </row>
-    <row r="254" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A254" s="4">
         <v>252</v>
       </c>
@@ -21675,7 +21666,7 @@
         <v>29.833025880740301</v>
       </c>
     </row>
-    <row r="255" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A255" s="4">
         <v>253</v>
       </c>
@@ -21757,7 +21748,7 @@
         <v>30.321430073304999</v>
       </c>
     </row>
-    <row r="256" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A256" s="4">
         <v>254</v>
       </c>
@@ -21839,7 +21830,7 @@
         <v>31.241288391566101</v>
       </c>
     </row>
-    <row r="257" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A257" s="4">
         <v>255</v>
       </c>
@@ -21921,7 +21912,7 @@
         <v>32.442144175962397</v>
       </c>
     </row>
-    <row r="258" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A258" s="4">
         <v>256</v>
       </c>
@@ -22003,7 +21994,7 @@
         <v>33.380723590489403</v>
       </c>
     </row>
-    <row r="259" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A259" s="4">
         <v>257</v>
       </c>
@@ -22085,7 +22076,7 @@
         <v>33.576693497222898</v>
       </c>
     </row>
-    <row r="260" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A260" s="4">
         <v>258</v>
       </c>
@@ -22167,7 +22158,7 @@
         <v>34.039171782289998</v>
       </c>
     </row>
-    <row r="261" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A261" s="4">
         <v>259</v>
       </c>
@@ -22249,7 +22240,7 @@
         <v>34.5633153964095</v>
       </c>
     </row>
-    <row r="262" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A262" s="4">
         <v>260</v>
       </c>
@@ -22331,7 +22322,7 @@
         <v>35.243272783614103</v>
       </c>
     </row>
-    <row r="263" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A263" s="4">
         <v>261</v>
       </c>
@@ -22413,7 +22404,7 @@
         <v>35.9498050617091</v>
       </c>
     </row>
-    <row r="264" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A264" s="4">
         <v>262</v>
       </c>
@@ -22495,7 +22486,7 @@
         <v>36.655447226794401</v>
       </c>
     </row>
-    <row r="265" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A265" s="4">
         <v>263</v>
       </c>
@@ -22577,7 +22568,7 @@
         <v>36.978448067860199</v>
       </c>
     </row>
-    <row r="266" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A266" s="4">
         <v>264</v>
       </c>
@@ -22659,7 +22650,7 @@
         <v>37.571222731222598</v>
       </c>
     </row>
-    <row r="267" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A267" s="4">
         <v>265</v>
       </c>
@@ -22741,7 +22732,7 @@
         <v>38.683797841457</v>
       </c>
     </row>
-    <row r="268" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A268" s="4">
         <v>266</v>
       </c>
@@ -22823,7 +22814,7 @@
         <v>40.108469578976297</v>
       </c>
     </row>
-    <row r="269" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A269" s="4">
         <v>267</v>
       </c>
@@ -22905,7 +22896,7 @@
         <v>41.669773300721502</v>
       </c>
     </row>
-    <row r="270" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A270" s="4">
         <v>268</v>
       </c>
@@ -22987,7 +22978,7 @@
         <v>43.355401407904203</v>
       </c>
     </row>
-    <row r="271" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A271" s="4">
         <v>269</v>
       </c>
@@ -23069,7 +23060,7 @@
         <v>45.0853097599989</v>
       </c>
     </row>
-    <row r="272" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A272" s="4">
         <v>270</v>
       </c>
@@ -23151,7 +23142,7 @@
         <v>44.8302113134135</v>
       </c>
     </row>
-    <row r="273" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A273" s="4">
         <v>271</v>
       </c>
@@ -23233,7 +23224,7 @@
         <v>44.682997203934796</v>
       </c>
     </row>
-    <row r="274" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A274" s="4">
         <v>272</v>
       </c>
@@ -23315,7 +23306,7 @@
         <v>44.800202646040198</v>
       </c>
     </row>
-    <row r="275" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A275" s="4">
         <v>273</v>
       </c>
@@ -23397,7 +23388,7 @@
         <v>43.949283404165698</v>
       </c>
     </row>
-    <row r="276" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A276" s="4">
         <v>274</v>
       </c>
@@ -23479,7 +23470,7 @@
         <v>44.595460482788901</v>
       </c>
     </row>
-    <row r="277" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A277" s="4">
         <v>275</v>
       </c>
@@ -23561,7 +23552,7 @@
         <v>45.489532518218297</v>
       </c>
     </row>
-    <row r="278" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A278" s="4">
         <v>276</v>
       </c>
@@ -23643,7 +23634,7 @@
         <v>45.917445996110096</v>
       </c>
     </row>
-    <row r="279" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A279" s="4">
         <v>277</v>
       </c>
@@ -23725,7 +23716,7 @@
         <v>47.073628957847298</v>
       </c>
     </row>
-    <row r="280" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A280" s="4">
         <v>278</v>
       </c>
@@ -23807,7 +23798,7 @@
         <v>48.402261377820203</v>
       </c>
     </row>
-    <row r="281" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A281" s="4">
         <v>279</v>
       </c>
@@ -23889,7 +23880,7 @@
         <v>49.253150487665899</v>
       </c>
     </row>
-    <row r="282" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A282" s="4">
         <v>280</v>
       </c>
@@ -23971,7 +23962,7 @@
         <v>50.043261803951097</v>
       </c>
     </row>
-    <row r="283" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A283" s="4">
         <v>281</v>
       </c>
@@ -24053,7 +24044,7 @@
         <v>50.482810002419299</v>
       </c>
     </row>
-    <row r="284" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A284" s="4">
         <v>282</v>
       </c>
@@ -24135,7 +24126,7 @@
         <v>50.524515847224599</v>
       </c>
     </row>
-    <row r="285" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A285" s="4">
         <v>283</v>
       </c>
@@ -24217,7 +24208,7 @@
         <v>48.9727311126397</v>
       </c>
     </row>
-    <row r="286" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A286" s="4">
         <v>284</v>
       </c>
@@ -24299,7 +24290,7 @@
         <v>47.489243388807999</v>
       </c>
     </row>
-    <row r="287" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A287" s="4">
         <v>285</v>
       </c>
@@ -24381,7 +24372,7 @@
         <v>45.988055235207099</v>
       </c>
     </row>
-    <row r="288" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A288" s="4">
         <v>286</v>
       </c>
@@ -24463,7 +24454,7 @@
         <v>43.458459724148398</v>
       </c>
     </row>
-    <row r="289" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A289" s="4">
         <v>287</v>
       </c>
@@ -24545,7 +24536,7 @@
         <v>42.336710251636497</v>
       </c>
     </row>
-    <row r="290" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A290" s="4">
         <v>288</v>
       </c>
@@ -24627,7 +24618,7 @@
         <v>41.204624480284501</v>
       </c>
     </row>
-    <row r="291" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A291" s="4">
         <v>289</v>
       </c>
@@ -24709,7 +24700,7 @@
         <v>39.703261507314402</v>
       </c>
     </row>
-    <row r="292" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A292" s="4">
         <v>290</v>
       </c>
@@ -24791,7 +24782,7 @@
         <v>39.186372254460899</v>
       </c>
     </row>
-    <row r="293" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A293" s="4">
         <v>291</v>
       </c>
@@ -24873,7 +24864,7 @@
         <v>39.364514982524398</v>
       </c>
     </row>
-    <row r="294" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A294" s="4">
         <v>292</v>
       </c>
@@ -24955,7 +24946,7 @@
         <v>39.162926652029299</v>
       </c>
     </row>
-    <row r="295" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A295" s="4">
         <v>293</v>
       </c>
@@ -25037,7 +25028,7 @@
         <v>38.5659328083131</v>
       </c>
     </row>
-    <row r="296" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A296" s="4">
         <v>294</v>
       </c>
@@ -25119,7 +25110,7 @@
         <v>37.502797409335997</v>
       </c>
     </row>
-    <row r="297" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A297" s="4">
         <v>295</v>
       </c>
@@ -25201,7 +25192,7 @@
         <v>36.244865030022403</v>
       </c>
     </row>
-    <row r="298" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A298" s="4">
         <v>296</v>
       </c>
@@ -25283,7 +25274,7 @@
         <v>34.674984555811697</v>
       </c>
     </row>
-    <row r="299" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A299" s="4">
         <v>297</v>
       </c>
@@ -25365,7 +25356,7 @@
         <v>33.072077162676301</v>
       </c>
     </row>
-    <row r="300" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A300" s="4">
         <v>298</v>
       </c>
@@ -25447,7 +25438,7 @@
         <v>31.572873004156001</v>
       </c>
     </row>
-    <row r="301" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A301" s="4">
         <v>299</v>
       </c>
@@ -25529,7 +25520,7 @@
         <v>29.9561712714073</v>
       </c>
     </row>
-    <row r="302" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A302" s="4">
         <v>300</v>
       </c>
@@ -25611,7 +25602,7 @@
         <v>28.400852893868699</v>
       </c>
     </row>
-    <row r="303" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A303" s="4">
         <v>301</v>
       </c>
@@ -25693,7 +25684,7 @@
         <v>26.600677803712301</v>
       </c>
     </row>
-    <row r="304" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A304" s="4">
         <v>302</v>
       </c>
@@ -25775,7 +25766,7 @@
         <v>24.9290866485671</v>
       </c>
     </row>
-    <row r="305" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A305" s="4">
         <v>303</v>
       </c>
@@ -25857,7 +25848,7 @@
         <v>24.330164002215401</v>
       </c>
     </row>
-    <row r="306" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A306" s="4">
         <v>304</v>
       </c>
@@ -25939,7 +25930,7 @@
         <v>24.249288733771099</v>
       </c>
     </row>
-    <row r="307" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A307" s="4">
         <v>305</v>
       </c>
@@ -26021,7 +26012,7 @@
         <v>24.012982288271299</v>
       </c>
     </row>
-    <row r="308" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A308" s="4">
         <v>306</v>
       </c>
@@ -26103,7 +26094,7 @@
         <v>24.021074651591999</v>
       </c>
     </row>
-    <row r="309" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A309" s="4">
         <v>307</v>
       </c>
@@ -26185,7 +26176,7 @@
         <v>24.3361205913288</v>
       </c>
     </row>
-    <row r="310" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A310" s="4">
         <v>308</v>
       </c>
@@ -26267,7 +26258,7 @@
         <v>24.6609309569155</v>
       </c>
     </row>
-    <row r="311" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A311" s="4">
         <v>309</v>
       </c>
@@ -26349,7 +26340,7 @@
         <v>24.609799024355802</v>
       </c>
     </row>
-    <row r="312" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A312" s="4">
         <v>310</v>
       </c>
@@ -26431,7 +26422,7 @@
         <v>24.299107490012901</v>
       </c>
     </row>
-    <row r="313" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A313" s="4">
         <v>311</v>
       </c>
@@ -26513,7 +26504,7 @@
         <v>23.708973109991799</v>
       </c>
     </row>
-    <row r="314" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A314" s="4">
         <v>312</v>
       </c>
@@ -26595,7 +26586,7 @@
         <v>23.320559083278098</v>
       </c>
     </row>
-    <row r="315" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A315" s="4">
         <v>313</v>
       </c>
@@ -26677,7 +26668,7 @@
         <v>23.114949305379099</v>
       </c>
     </row>
-    <row r="316" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A316" s="4">
         <v>314</v>
       </c>
@@ -26759,7 +26750,7 @@
         <v>22.4902681345764</v>
       </c>
     </row>
-    <row r="317" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A317" s="4">
         <v>315</v>
       </c>
@@ -26841,7 +26832,7 @@
         <v>21.5965931053479</v>
       </c>
     </row>
-    <row r="318" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A318" s="4">
         <v>316</v>
       </c>
@@ -26923,7 +26914,7 @@
         <v>21.920946856281098</v>
       </c>
     </row>
-    <row r="319" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A319" s="4">
         <v>317</v>
       </c>
@@ -27005,7 +26996,7 @@
         <v>22.2221324821477</v>
       </c>
     </row>
-    <row r="320" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A320" s="4">
         <v>318</v>
       </c>
@@ -27087,7 +27078,7 @@
         <v>22.075075981773001</v>
       </c>
     </row>
-    <row r="321" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A321" s="4">
         <v>319</v>
       </c>
@@ -27169,7 +27160,7 @@
         <v>22.5758479738234</v>
       </c>
     </row>
-    <row r="322" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A322" s="4">
         <v>320</v>
       </c>
@@ -27251,7 +27242,7 @@
         <v>23.204105080850901</v>
       </c>
     </row>
-    <row r="323" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A323" s="4">
         <v>321</v>
       </c>
@@ -27333,7 +27324,7 @@
         <v>23.831982200405601</v>
       </c>
     </row>
-    <row r="324" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A324" s="4">
         <v>322</v>
       </c>
@@ -27415,7 +27406,7 @@
         <v>24.100669583639199</v>
       </c>
     </row>
-    <row r="325" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A325" s="4">
         <v>323</v>
       </c>
@@ -27497,7 +27488,7 @@
         <v>23.957310799270498</v>
       </c>
     </row>
-    <row r="326" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A326" s="4">
         <v>324</v>
       </c>
@@ -27579,7 +27570,7 @@
         <v>23.347236408235101</v>
       </c>
     </row>
-    <row r="327" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A327" s="4">
         <v>325</v>
       </c>
@@ -27661,7 +27652,7 @@
         <v>23.465210872016701</v>
       </c>
     </row>
-    <row r="328" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A328" s="4">
         <v>326</v>
       </c>
@@ -27743,7 +27734,7 @@
         <v>23.819705472483701</v>
       </c>
     </row>
-    <row r="329" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A329" s="4">
         <v>327</v>
       </c>
@@ -27825,7 +27816,7 @@
         <v>23.716015492394899</v>
       </c>
     </row>
-    <row r="330" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A330" s="4">
         <v>328</v>
       </c>
@@ -27907,7 +27898,7 @@
         <v>23.7268905067628</v>
       </c>
     </row>
-    <row r="331" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A331" s="4">
         <v>329</v>
       </c>
@@ -27989,7 +27980,7 @@
         <v>24.308211406051001</v>
       </c>
     </row>
-    <row r="332" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A332" s="4">
         <v>330</v>
       </c>
@@ -28071,7 +28062,7 @@
         <v>24.296009563747699</v>
       </c>
     </row>
-    <row r="333" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A333" s="4">
         <v>331</v>
       </c>
@@ -28153,7 +28144,7 @@
         <v>24.0975316290112</v>
       </c>
     </row>
-    <row r="334" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A334" s="4">
         <v>332</v>
       </c>
@@ -28235,7 +28226,7 @@
         <v>24.040589746413101</v>
       </c>
     </row>
-    <row r="335" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A335" s="4">
         <v>333</v>
       </c>
@@ -28317,7 +28308,7 @@
         <v>24.040297779885101</v>
       </c>
     </row>
-    <row r="336" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A336" s="4">
         <v>334</v>
       </c>
@@ -28399,7 +28390,7 @@
         <v>24.0358557453396</v>
       </c>
     </row>
-    <row r="337" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A337" s="4">
         <v>335</v>
       </c>
@@ -28481,7 +28472,7 @@
         <v>24.3059452059323</v>
       </c>
     </row>
-    <row r="338" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A338" s="4">
         <v>336</v>
       </c>
@@ -28563,7 +28554,7 @@
         <v>23.5333877332789</v>
       </c>
     </row>
-    <row r="339" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A339" s="4">
         <v>337</v>
       </c>
@@ -28645,7 +28636,7 @@
         <v>22.5567838939</v>
       </c>
     </row>
-    <row r="340" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A340" s="4">
         <v>338</v>
       </c>
@@ -28727,7 +28718,7 @@
         <v>22.037988007839701</v>
       </c>
     </row>
-    <row r="341" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A341" s="4">
         <v>339</v>
       </c>
@@ -28809,7 +28800,7 @@
         <v>21.400084393895899</v>
       </c>
     </row>
-    <row r="342" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A342" s="4">
         <v>340</v>
       </c>
@@ -28891,7 +28882,7 @@
         <v>20.774055296181899</v>
       </c>
     </row>
-    <row r="343" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A343" s="4">
         <v>341</v>
       </c>
@@ -28973,7 +28964,7 @@
         <v>20.713454193698698</v>
       </c>
     </row>
-    <row r="344" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A344" s="4">
         <v>342</v>
       </c>
@@ -29055,7 +29046,7 @@
         <v>20.820641487708102</v>
       </c>
     </row>
-    <row r="345" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A345" s="4">
         <v>343</v>
       </c>
@@ -29137,7 +29128,7 @@
         <v>20.007212094078799</v>
       </c>
     </row>
-    <row r="346" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A346" s="4">
         <v>344</v>
       </c>
@@ -29219,7 +29210,7 @@
         <v>19.400862031148701</v>
       </c>
     </row>
-    <row r="347" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A347" s="4">
         <v>345</v>
       </c>
@@ -29301,7 +29292,7 @@
         <v>19.033849901852602</v>
       </c>
     </row>
-    <row r="348" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A348" s="4">
         <v>346</v>
       </c>
@@ -29383,7 +29374,7 @@
         <v>18.916167065472699</v>
       </c>
     </row>
-    <row r="349" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A349" s="4">
         <v>347</v>
       </c>
@@ -29465,7 +29456,7 @@
         <v>18.9864164410826</v>
       </c>
     </row>
-    <row r="350" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A350" s="4">
         <v>348</v>
       </c>
@@ -29547,7 +29538,7 @@
         <v>19.4721973298854</v>
       </c>
     </row>
-    <row r="351" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A351" s="4">
         <v>349</v>
       </c>
@@ -29629,7 +29620,7 @@
         <v>19.065660266944601</v>
       </c>
     </row>
-    <row r="352" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A352" s="4">
         <v>350</v>
       </c>
@@ -29711,7 +29702,7 @@
         <v>18.450557253607801</v>
       </c>
     </row>
-    <row r="353" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A353" s="4">
         <v>351</v>
       </c>
@@ -29793,7 +29784,7 @@
         <v>17.993188939884899</v>
       </c>
     </row>
-    <row r="354" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A354" s="4">
         <v>352</v>
       </c>
@@ -29875,7 +29866,7 @@
         <v>17.370528133367301</v>
       </c>
     </row>
-    <row r="355" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A355" s="4">
         <v>353</v>
       </c>
@@ -29957,7 +29948,7 @@
         <v>16.361103887229799</v>
       </c>
     </row>
-    <row r="356" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A356" s="4">
         <v>354</v>
       </c>
@@ -30039,7 +30030,7 @@
         <v>15.552843087417999</v>
       </c>
     </row>
-    <row r="357" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A357" s="4">
         <v>355</v>
       </c>
@@ -30121,7 +30112,7 @@
         <v>14.9670865577054</v>
       </c>
     </row>
-    <row r="358" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A358" s="4">
         <v>356</v>
       </c>
@@ -30203,7 +30194,7 @@
         <v>14.2776973816188</v>
       </c>
     </row>
-    <row r="359" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A359" s="4">
         <v>357</v>
       </c>
@@ -30285,7 +30276,7 @@
         <v>13.8608899240038</v>
       </c>
     </row>
-    <row r="360" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A360" s="4">
         <v>358</v>
       </c>
@@ -30367,7 +30358,7 @@
         <v>13.8678426711318</v>
       </c>
     </row>
-    <row r="361" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A361" s="4">
         <v>359</v>
       </c>
@@ -30449,7 +30440,7 @@
         <v>13.9525434693052</v>
       </c>
     </row>
-    <row r="362" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A362" s="4">
         <v>360</v>
       </c>
@@ -30531,7 +30522,7 @@
         <v>14.3228300719055</v>
       </c>
     </row>
-    <row r="363" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A363" s="4">
         <v>361</v>
       </c>
@@ -30613,7 +30604,7 @@
         <v>14.884309733596799</v>
       </c>
     </row>
-    <row r="364" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A364" s="4">
         <v>362</v>
       </c>
@@ -30695,7 +30686,7 @@
         <v>15.1235247980179</v>
       </c>
     </row>
-    <row r="365" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A365" s="4">
         <v>363</v>
       </c>
@@ -30777,7 +30768,7 @@
         <v>15.190511916975399</v>
       </c>
     </row>
-    <row r="366" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A366" s="4">
         <v>364</v>
       </c>
@@ -30859,7 +30850,7 @@
         <v>15.2527142417217</v>
       </c>
     </row>
-    <row r="367" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A367" s="4">
         <v>365</v>
       </c>
@@ -30941,7 +30932,7 @@
         <v>15.064245297757999</v>
       </c>
     </row>
-    <row r="368" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A368" s="4">
         <v>366</v>
       </c>
@@ -31023,7 +31014,7 @@
         <v>14.4087144661494</v>
       </c>
     </row>
-    <row r="369" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A369" s="4">
         <v>367</v>
       </c>
@@ -31105,7 +31096,7 @@
         <v>13.5452486298121</v>
       </c>
     </row>
-    <row r="370" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A370" s="4">
         <v>368</v>
       </c>
@@ -31187,7 +31178,7 @@
         <v>12.9272276871381</v>
       </c>
     </row>
-    <row r="371" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A371" s="4">
         <v>369</v>
       </c>
@@ -31269,7 +31260,7 @@
         <v>12.6547212717257</v>
       </c>
     </row>
-    <row r="372" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A372" s="4">
         <v>370</v>
       </c>
@@ -31351,7 +31342,7 @@
         <v>12.4603744291437</v>
       </c>
     </row>
-    <row r="373" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A373" s="4">
         <v>371</v>
       </c>
@@ -31433,7 +31424,7 @@
         <v>13.563590916138001</v>
       </c>
     </row>
-    <row r="374" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A374" s="4">
         <v>372</v>
       </c>
@@ -31515,7 +31506,7 @@
         <v>14.7019891631258</v>
       </c>
     </row>
-    <row r="375" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A375" s="4">
         <v>373</v>
       </c>
@@ -31597,7 +31588,7 @@
         <v>15.972210649169</v>
       </c>
     </row>
-    <row r="376" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A376" s="4">
         <v>374</v>
       </c>
@@ -31679,7 +31670,7 @@
         <v>17.4146380538457</v>
       </c>
     </row>
-    <row r="377" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A377" s="4">
         <v>375</v>
       </c>
@@ -31761,7 +31752,7 @@
         <v>18.168954250697599</v>
       </c>
     </row>
-    <row r="378" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A378" s="4">
         <v>376</v>
       </c>
@@ -31843,7 +31834,7 @@
         <v>19.023318463398201</v>
       </c>
     </row>
-    <row r="379" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A379" s="4">
         <v>377</v>
       </c>
@@ -31925,7 +31916,7 @@
         <v>19.565028793365201</v>
       </c>
     </row>
-    <row r="380" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A380" s="4">
         <v>378</v>
       </c>
@@ -32007,7 +31998,7 @@
         <v>19.562903121324101</v>
       </c>
     </row>
-    <row r="381" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A381" s="4">
         <v>379</v>
       </c>
@@ -32089,7 +32080,7 @@
         <v>18.794050732586101</v>
       </c>
     </row>
-    <row r="382" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A382" s="4">
         <v>380</v>
       </c>
@@ -32171,7 +32162,7 @@
         <v>17.636341940310299</v>
       </c>
     </row>
-    <row r="383" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A383" s="4">
         <v>381</v>
       </c>
@@ -32253,7 +32244,7 @@
         <v>16.8959692304635</v>
       </c>
     </row>
-    <row r="384" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A384" s="4">
         <v>382</v>
       </c>
@@ -32335,7 +32326,7 @@
         <v>15.9743349349905</v>
       </c>
     </row>
-    <row r="385" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A385" s="4">
         <v>383</v>
       </c>
@@ -32417,7 +32408,7 @@
         <v>15.378211183727</v>
       </c>
     </row>
-    <row r="386" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A386" s="4">
         <v>384</v>
       </c>
@@ -32499,7 +32490,7 @@
         <v>15.8727196009918</v>
       </c>
     </row>
-    <row r="387" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A387" s="4">
         <v>385</v>
       </c>
@@ -32581,7 +32572,7 @@
         <v>16.331905988451901</v>
       </c>
     </row>
-    <row r="388" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A388" s="4">
         <v>386</v>
       </c>
@@ -32663,7 +32654,7 @@
         <v>17.1822329095613</v>
       </c>
     </row>
-    <row r="389" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A389" s="4">
         <v>387</v>
       </c>
@@ -32745,7 +32736,7 @@
         <v>18.110362038823698</v>
       </c>
     </row>
-    <row r="390" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A390" s="4">
         <v>388</v>
       </c>
@@ -32827,7 +32818,7 @@
         <v>18.2596895435288</v>
       </c>
     </row>
-    <row r="391" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A391" s="4">
         <v>389</v>
       </c>
@@ -32909,7 +32900,7 @@
         <v>18.666597694851198</v>
       </c>
     </row>
-    <row r="392" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A392" s="4">
         <v>390</v>
       </c>
@@ -32991,7 +32982,7 @@
         <v>18.6654025041172</v>
       </c>
     </row>
-    <row r="393" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A393" s="4">
         <v>391</v>
       </c>
@@ -33073,7 +33064,7 @@
         <v>19.074902798161101</v>
       </c>
     </row>
-    <row r="394" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A394" s="4">
         <v>392</v>
       </c>
@@ -33155,7 +33146,7 @@
         <v>19.123796163093498</v>
       </c>
     </row>
-    <row r="395" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A395" s="4">
         <v>393</v>
       </c>
@@ -33237,7 +33228,7 @@
         <v>19.009303941781699</v>
       </c>
     </row>
-    <row r="396" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A396" s="4">
         <v>394</v>
       </c>
@@ -33319,7 +33310,7 @@
         <v>18.307842361126099</v>
       </c>
     </row>
-    <row r="397" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A397" s="4">
         <v>395</v>
       </c>
@@ -33401,7 +33392,7 @@
         <v>17.0879358103426</v>
       </c>
     </row>
-    <row r="398" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A398" s="4">
         <v>396</v>
       </c>
@@ -33483,7 +33474,7 @@
         <v>16.290524284807301</v>
       </c>
     </row>
-    <row r="399" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A399" s="4">
         <v>397</v>
       </c>
@@ -33565,7 +33556,7 @@
         <v>15.575556265207601</v>
       </c>
     </row>
-    <row r="400" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A400" s="4">
         <v>398</v>
       </c>
@@ -33647,7 +33638,7 @@
         <v>14.974989311149301</v>
       </c>
     </row>
-    <row r="401" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A401" s="4">
         <v>399</v>
       </c>
@@ -33729,7 +33720,7 @@
         <v>14.592319179051501</v>
       </c>
     </row>
-    <row r="402" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A402" s="4">
         <v>400</v>
       </c>
@@ -33811,7 +33802,7 @@
         <v>14.6044250109464</v>
       </c>
     </row>
-    <row r="403" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A403" s="4">
         <v>401</v>
       </c>
@@ -33893,7 +33884,7 @@
         <v>14.670969027999099</v>
       </c>
     </row>
-    <row r="404" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A404" s="4">
         <v>402</v>
       </c>
@@ -33975,7 +33966,7 @@
         <v>14.641936624316999</v>
       </c>
     </row>
-    <row r="405" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A405" s="4">
         <v>403</v>
       </c>
@@ -34057,7 +34048,7 @@
         <v>14.501903250587301</v>
       </c>
     </row>
-    <row r="406" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A406" s="4">
         <v>404</v>
       </c>
@@ -34139,7 +34130,7 @@
         <v>14.408782776300701</v>
       </c>
     </row>
-    <row r="407" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A407" s="4">
         <v>405</v>
       </c>
@@ -34221,7 +34212,7 @@
         <v>14.787537026659299</v>
       </c>
     </row>
-    <row r="408" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A408" s="4">
         <v>406</v>
       </c>
@@ -34303,7 +34294,7 @@
         <v>15.136210145418</v>
       </c>
     </row>
-    <row r="409" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A409" s="4">
         <v>407</v>
       </c>
@@ -34385,7 +34376,7 @@
         <v>15.197387871054801</v>
       </c>
     </row>
-    <row r="410" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A410" s="4">
         <v>408</v>
       </c>
@@ -34467,7 +34458,7 @@
         <v>14.3193647860939</v>
       </c>
     </row>
-    <row r="411" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A411" s="4">
         <v>409</v>
       </c>
@@ -34549,7 +34540,7 @@
         <v>13.455772188056899</v>
       </c>
     </row>
-    <row r="412" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A412" s="4">
         <v>410</v>
       </c>
@@ -34631,7 +34622,7 @@
         <v>12.6872116218054</v>
       </c>
     </row>
-    <row r="413" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A413" s="4">
         <v>411</v>
       </c>
@@ -34713,7 +34704,7 @@
         <v>12.3476066811418</v>
       </c>
     </row>
-    <row r="414" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A414" s="4">
         <v>412</v>
       </c>
@@ -34795,7 +34786,7 @@
         <v>11.958458425863901</v>
       </c>
     </row>
-    <row r="415" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A415" s="4">
         <v>413</v>
       </c>
@@ -34877,7 +34868,7 @@
         <v>11.9543942276407</v>
       </c>
     </row>
-    <row r="416" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A416" s="4">
         <v>414</v>
       </c>
@@ -34959,7 +34950,7 @@
         <v>12.346677481393</v>
       </c>
     </row>
-    <row r="417" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A417" s="4">
         <v>415</v>
       </c>
@@ -35041,7 +35032,7 @@
         <v>13.0859098694095</v>
       </c>
     </row>
-    <row r="418" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A418" s="4">
         <v>416</v>
       </c>
@@ -35123,7 +35114,7 @@
         <v>13.880547133235901</v>
       </c>
     </row>
-    <row r="419" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A419" s="4">
         <v>417</v>
       </c>
@@ -35205,7 +35196,7 @@
         <v>14.4148382275316</v>
       </c>
     </row>
-    <row r="420" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A420" s="4">
         <v>418</v>
       </c>
@@ -35287,7 +35278,7 @@
         <v>14.957807606987</v>
       </c>
     </row>
-    <row r="421" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A421" s="4">
         <v>419</v>
       </c>
@@ -35369,7 +35360,7 @@
         <v>15.3296561037263</v>
       </c>
     </row>
-    <row r="422" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A422" s="4">
         <v>420</v>
       </c>
@@ -35451,7 +35442,7 @@
         <v>15.968613297333301</v>
       </c>
     </row>
-    <row r="423" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A423" s="4">
         <v>421</v>
       </c>
@@ -35533,7 +35524,7 @@
         <v>15.587223497216399</v>
       </c>
     </row>
-    <row r="424" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A424" s="4">
         <v>422</v>
       </c>
@@ -35615,7 +35606,7 @@
         <v>14.807751837768199</v>
       </c>
     </row>
-    <row r="425" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A425" s="4">
         <v>423</v>
       </c>
@@ -35697,7 +35688,7 @@
         <v>14.0858205828425</v>
       </c>
     </row>
-    <row r="426" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A426" s="4">
         <v>424</v>
       </c>
@@ -35779,7 +35770,7 @@
         <v>13.8267905444765</v>
       </c>
     </row>
-    <row r="427" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A427" s="4">
         <v>425</v>
       </c>
@@ -35861,7 +35852,7 @@
         <v>13.239849190144</v>
       </c>
     </row>
-    <row r="428" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A428" s="4">
         <v>426</v>
       </c>
@@ -35943,7 +35934,7 @@
         <v>12.8184044512486</v>
       </c>
     </row>
-    <row r="429" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A429" s="4">
         <v>427</v>
       </c>
@@ -36025,7 +36016,7 @@
         <v>12.9848088164429</v>
       </c>
     </row>
-    <row r="430" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A430" s="4">
         <v>428</v>
       </c>
@@ -36107,7 +36098,7 @@
         <v>13.6733974281626</v>
       </c>
     </row>
-    <row r="431" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A431" s="4">
         <v>429</v>
       </c>
@@ -36189,7 +36180,7 @@
         <v>14.0396838581923</v>
       </c>
     </row>
-    <row r="432" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A432" s="4">
         <v>430</v>
       </c>
@@ -36271,7 +36262,7 @@
         <v>14.830533018637199</v>
       </c>
     </row>
-    <row r="433" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A433" s="4">
         <v>431</v>
       </c>
@@ -36353,7 +36344,7 @@
         <v>15.504727933627199</v>
       </c>
     </row>
-    <row r="434" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A434" s="4">
         <v>432</v>
       </c>
@@ -36435,7 +36426,7 @@
         <v>16.6004438243355</v>
       </c>
     </row>
-    <row r="435" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A435" s="4">
         <v>433</v>
       </c>
@@ -36517,7 +36508,7 @@
         <v>17.520967675199099</v>
       </c>
     </row>
-    <row r="436" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A436" s="4">
         <v>434</v>
       </c>
@@ -36599,7 +36590,7 @@
         <v>17.5201980007906</v>
       </c>
     </row>
-    <row r="437" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A437" s="4">
         <v>435</v>
       </c>
@@ -36681,7 +36672,7 @@
         <v>17.258230265366201</v>
       </c>
     </row>
-    <row r="438" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A438" s="4">
         <v>436</v>
       </c>
@@ -36763,7 +36754,7 @@
         <v>16.526766103900702</v>
       </c>
     </row>
-    <row r="439" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A439" s="4">
         <v>437</v>
       </c>
@@ -36845,7 +36836,7 @@
         <v>15.948157559890999</v>
       </c>
     </row>
-    <row r="440" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A440" s="4">
         <v>438</v>
       </c>
@@ -36927,7 +36918,7 @@
         <v>15.0443602217851</v>
       </c>
     </row>
-    <row r="441" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A441" s="4">
         <v>439</v>
       </c>
@@ -37009,7 +37000,7 @@
         <v>14.787644812962601</v>
       </c>
     </row>
-    <row r="442" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A442" s="4">
         <v>440</v>
       </c>
@@ -37091,7 +37082,7 @@
         <v>14.929267156716</v>
       </c>
     </row>
-    <row r="443" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A443" s="4">
         <v>441</v>
       </c>
@@ -37173,7 +37164,7 @@
         <v>15.363294955236601</v>
       </c>
     </row>
-    <row r="444" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A444" s="4">
         <v>442</v>
       </c>
@@ -37255,7 +37246,7 @@
         <v>14.755581750279401</v>
       </c>
     </row>
-    <row r="445" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A445" s="4">
         <v>443</v>
       </c>
@@ -37337,7 +37328,7 @@
         <v>14.7586480006429</v>
       </c>
     </row>
-    <row r="446" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A446" s="4">
         <v>444</v>
       </c>
@@ -37419,7 +37410,7 @@
         <v>14.951896562116101</v>
       </c>
     </row>
-    <row r="447" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A447" s="4">
         <v>445</v>
       </c>
@@ -37501,7 +37492,7 @@
         <v>15.5170034839955</v>
       </c>
     </row>
-    <row r="448" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A448" s="4">
         <v>446</v>
       </c>
@@ -37583,7 +37574,7 @@
         <v>17.431205146225601</v>
       </c>
     </row>
-    <row r="449" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A449" s="4">
         <v>447</v>
       </c>
@@ -37665,7 +37656,7 @@
         <v>19.1206474373075</v>
       </c>
     </row>
-    <row r="450" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A450" s="4">
         <v>448</v>
       </c>
@@ -37747,7 +37738,7 @@
         <v>20.7295214615167</v>
       </c>
     </row>
-    <row r="451" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A451" s="4">
         <v>449</v>
       </c>
@@ -37829,7 +37820,7 @@
         <v>21.8309555281553</v>
       </c>
     </row>
-    <row r="452" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A452" s="4">
         <v>450</v>
       </c>
@@ -37911,7 +37902,7 @@
         <v>21.9815681323878</v>
       </c>
     </row>
-    <row r="453" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A453" s="4">
         <v>451</v>
       </c>
@@ -37993,7 +37984,7 @@
         <v>21.994878157898899</v>
       </c>
     </row>
-    <row r="454" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A454" s="4">
         <v>452</v>
       </c>
@@ -38075,7 +38066,7 @@
         <v>22.736988437650801</v>
       </c>
     </row>
-    <row r="455" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A455" s="4">
         <v>453</v>
       </c>
@@ -38157,7 +38148,7 @@
         <v>23.426090840277599</v>
       </c>
     </row>
-    <row r="456" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A456" s="4">
         <v>454</v>
       </c>
@@ -38239,7 +38230,7 @@
         <v>24.3922916910028</v>
       </c>
     </row>
-    <row r="457" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A457" s="4">
         <v>455</v>
       </c>
@@ -38321,7 +38312,7 @@
         <v>25.052390563449102</v>
       </c>
     </row>
-    <row r="458" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A458" s="4">
         <v>456</v>
       </c>
@@ -38403,7 +38394,7 @@
         <v>26.2077623299962</v>
       </c>
     </row>
-    <row r="459" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A459" s="4">
         <v>457</v>
       </c>
@@ -38485,7 +38476,7 @@
         <v>27.435884325085102</v>
       </c>
     </row>
-    <row r="460" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A460" s="4">
         <v>458</v>
       </c>
@@ -38567,7 +38558,7 @@
         <v>28.5370556655485</v>
       </c>
     </row>
-    <row r="461" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A461" s="4">
         <v>459</v>
       </c>
@@ -38649,7 +38640,7 @@
         <v>30.907045423627299</v>
       </c>
     </row>
-    <row r="462" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A462" s="4">
         <v>460</v>
       </c>
@@ -38731,7 +38722,7 @@
         <v>33.586863040948401</v>
       </c>
     </row>
-    <row r="463" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A463" s="4">
         <v>461</v>
       </c>
@@ -38813,7 +38804,7 @@
         <v>35.035803606518698</v>
       </c>
     </row>
-    <row r="464" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A464" s="4">
         <v>462</v>
       </c>
@@ -38895,7 +38886,7 @@
         <v>36.293336032319701</v>
       </c>
     </row>
-    <row r="465" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A465" s="4">
         <v>463</v>
       </c>
@@ -38977,7 +38968,7 @@
         <v>36.319274648816197</v>
       </c>
     </row>
-    <row r="466" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A466" s="4">
         <v>464</v>
       </c>
@@ -39059,7 +39050,7 @@
         <v>36.2749183166666</v>
       </c>
     </row>
-    <row r="467" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A467" s="4">
         <v>465</v>
       </c>
@@ -39141,7 +39132,7 @@
         <v>36.221345245740899</v>
       </c>
     </row>
-    <row r="468" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A468" s="4">
         <v>466</v>
       </c>
@@ -39223,7 +39214,7 @@
         <v>35.285229299660898</v>
       </c>
     </row>
-    <row r="469" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A469" s="4">
         <v>467</v>
       </c>
@@ -39305,7 +39296,7 @@
         <v>34.491844671828403</v>
       </c>
     </row>
-    <row r="470" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A470" s="4">
         <v>468</v>
       </c>
@@ -39387,7 +39378,7 @@
         <v>34.539741210403903</v>
       </c>
     </row>
-    <row r="471" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A471" s="4">
         <v>469</v>
       </c>
@@ -39469,7 +39460,7 @@
         <v>35.215494782381597</v>
       </c>
     </row>
-    <row r="472" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A472" s="4">
         <v>470</v>
       </c>
@@ -39551,7 +39542,7 @@
         <v>35.912930159901897</v>
       </c>
     </row>
-    <row r="473" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A473" s="4">
         <v>471</v>
       </c>
@@ -39633,7 +39624,7 @@
         <v>36.983497102724797</v>
       </c>
     </row>
-    <row r="474" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A474" s="4">
         <v>472</v>
       </c>
@@ -39715,7 +39706,7 @@
         <v>38.187671721008201</v>
       </c>
     </row>
-    <row r="475" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A475" s="4">
         <v>473</v>
       </c>
@@ -39797,7 +39788,7 @@
         <v>39.099087402643597</v>
       </c>
     </row>
-    <row r="476" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A476" s="4">
         <v>474</v>
       </c>
@@ -39879,7 +39870,7 @@
         <v>39.172245084957801</v>
       </c>
     </row>
-    <row r="477" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A477" s="4">
         <v>475</v>
       </c>
@@ -39961,7 +39952,7 @@
         <v>39.492990098616197</v>
       </c>
     </row>
-    <row r="478" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A478" s="4">
         <v>476</v>
       </c>
@@ -40043,7 +40034,7 @@
         <v>39.496202088094599</v>
       </c>
     </row>
-    <row r="479" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A479" s="4">
         <v>477</v>
       </c>
@@ -40125,7 +40116,7 @@
         <v>39.624171734112402</v>
       </c>
     </row>
-    <row r="480" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A480" s="4">
         <v>478</v>
       </c>
@@ -40207,7 +40198,7 @@
         <v>38.991812702546298</v>
       </c>
     </row>
-    <row r="481" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A481" s="4">
         <v>479</v>
       </c>
@@ -40289,7 +40280,7 @@
         <v>37.411146186790901</v>
       </c>
     </row>
-    <row r="482" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A482" s="4">
         <v>480</v>
       </c>
@@ -40371,7 +40362,7 @@
         <v>35.048205196674999</v>
       </c>
     </row>
-    <row r="483" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A483" s="4">
         <v>481</v>
       </c>
@@ -40453,7 +40444,7 @@
         <v>33.114286217894701</v>
       </c>
     </row>
-    <row r="484" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A484" s="4">
         <v>482</v>
       </c>
@@ -40535,7 +40526,7 @@
         <v>31.660245288681502</v>
       </c>
     </row>
-    <row r="485" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A485" s="4">
         <v>483</v>
       </c>
@@ -40617,7 +40608,7 @@
         <v>30.7003919657691</v>
       </c>
     </row>
-    <row r="486" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A486" s="4">
         <v>484</v>
       </c>
@@ -40699,7 +40690,7 @@
         <v>30.074803034748701</v>
       </c>
     </row>
-    <row r="487" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A487" s="4">
         <v>485</v>
       </c>
@@ -40781,7 +40772,7 @@
         <v>30.169507806168099</v>
       </c>
     </row>
-    <row r="488" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A488" s="4">
         <v>486</v>
       </c>
@@ -40863,7 +40854,7 @@
         <v>29.910825236138699</v>
       </c>
     </row>
-    <row r="489" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A489" s="4">
         <v>487</v>
       </c>
@@ -40945,7 +40936,7 @@
         <v>30.2008063990999</v>
       </c>
     </row>
-    <row r="490" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A490" s="4">
         <v>488</v>
       </c>
@@ -41027,7 +41018,7 @@
         <v>30.505063722257201</v>
       </c>
     </row>
-    <row r="491" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A491" s="4">
         <v>489</v>
       </c>
@@ -41109,7 +41100,7 @@
         <v>30.638516125959701</v>
       </c>
     </row>
-    <row r="492" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A492" s="4">
         <v>490</v>
       </c>
@@ -41191,7 +41182,7 @@
         <v>30.983166642136901</v>
       </c>
     </row>
-    <row r="493" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A493" s="4">
         <v>491</v>
       </c>
@@ -41273,7 +41264,7 @@
         <v>31.0967744154316</v>
       </c>
     </row>
-    <row r="494" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A494" s="4">
         <v>492</v>
       </c>
@@ -41355,7 +41346,7 @@
         <v>31.463819131952899</v>
       </c>
     </row>
-    <row r="495" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A495" s="4">
         <v>493</v>
       </c>
@@ -41437,7 +41428,7 @@
         <v>30.938772501267199</v>
       </c>
     </row>
-    <row r="496" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A496" s="4">
         <v>494</v>
       </c>
@@ -41519,7 +41510,7 @@
         <v>30.535927713522199</v>
       </c>
     </row>
-    <row r="497" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A497" s="4">
         <v>495</v>
       </c>
@@ -41601,7 +41592,7 @@
         <v>30.282776040365199</v>
       </c>
     </row>
-    <row r="498" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A498" s="4">
         <v>496</v>
       </c>
@@ -41683,7 +41674,7 @@
         <v>30.497836595735201</v>
       </c>
     </row>
-    <row r="499" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A499" s="4">
         <v>497</v>
       </c>
@@ -41765,7 +41756,7 @@
         <v>30.912779117799101</v>
       </c>
     </row>
-    <row r="500" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A500" s="4">
         <v>498</v>
       </c>
@@ -41847,7 +41838,7 @@
         <v>31.2099596113381</v>
       </c>
     </row>
-    <row r="501" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A501" s="4">
         <v>499</v>
       </c>
@@ -41929,7 +41920,7 @@
         <v>31.113824222237</v>
       </c>
     </row>
-    <row r="502" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A502" s="4">
         <v>500</v>
       </c>
@@ -42011,7 +42002,7 @@
         <v>30.960371035230398</v>
       </c>
     </row>
-    <row r="503" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A503" s="4">
         <v>501</v>
       </c>
@@ -42059,7 +42050,7 @@
         <f>100*testdata[[#This Row],[-DM14]]/testdata[[#This Row],[TR14]]</f>
         <v>31.150968674636061</v>
       </c>
-      <c r="N503" s="6">
+      <c r="N503" s="11">
         <f>100*ABS(testdata[[#This Row],[+DI14]]-testdata[[#This Row],[-DI14]])/(testdata[[#This Row],[+DI14]]+testdata[[#This Row],[-DI14]])</f>
         <v>27.387308306629919</v>
       </c>

</xml_diff>